<commit_message>
Updated script and source data (xlsx)
-new URL for the Eu scrapping data
-new versions of the source (transport) and intermediate xlsx
</commit_message>
<xml_diff>
--- a/data/emissions/sources/emissions_historical_latest.xlsx
+++ b/data/emissions/sources/emissions_historical_latest.xlsx
@@ -585,7 +585,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AK74"/>
+  <dimension ref="A1:AL74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A72" sqref="A72"/>
@@ -713,112 +713,115 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>15842.06810608921</v>
+        <v>15863.24954147978</v>
       </c>
       <c r="C2" t="n">
-        <v>15084.06583792503</v>
+        <v>15105.07311789158</v>
       </c>
       <c r="D2" t="n">
-        <v>14603.33286283946</v>
+        <v>14623.53841716949</v>
       </c>
       <c r="E2" t="n">
-        <v>14454.61508686201</v>
+        <v>14473.22074734073</v>
       </c>
       <c r="F2" t="n">
-        <v>14403.08965994239</v>
+        <v>14422.97565731601</v>
       </c>
       <c r="G2" t="n">
-        <v>12700.24487375463</v>
+        <v>12714.57920627653</v>
       </c>
       <c r="H2" t="n">
-        <v>12568.57366190546</v>
+        <v>12586.60283603493</v>
       </c>
       <c r="I2" t="n">
-        <v>12804.00808312036</v>
+        <v>12827.54701672393</v>
       </c>
       <c r="J2" t="n">
-        <v>13032.08738630091</v>
+        <v>13046.31802642162</v>
       </c>
       <c r="K2" t="n">
-        <v>13727.2568704113</v>
+        <v>13737.6418452229</v>
       </c>
       <c r="L2" t="n">
-        <v>13754.33578914839</v>
+        <v>13750.14481895911</v>
       </c>
       <c r="M2" t="n">
-        <v>14083.10475392134</v>
+        <v>14076.98704216207</v>
       </c>
       <c r="N2" t="n">
-        <v>13536.54985178814</v>
+        <v>13519.52562015265</v>
       </c>
       <c r="O2" t="n">
-        <v>12884.62389611392</v>
+        <v>12860.29509087484</v>
       </c>
       <c r="P2" t="n">
-        <v>12568.62715236548</v>
+        <v>12538.92442331814</v>
       </c>
       <c r="Q2" t="n">
-        <v>13791.49541373714</v>
+        <v>13757.20063514733</v>
       </c>
       <c r="R2" t="n">
-        <v>12952.96434756336</v>
+        <v>12910.37014793839</v>
       </c>
       <c r="S2" t="n">
-        <v>12928.29364881052</v>
+        <v>12902.72404099427</v>
       </c>
       <c r="T2" t="n">
-        <v>13201.20872739665</v>
+        <v>13154.4424235296</v>
       </c>
       <c r="U2" t="n">
-        <v>13418.80468991817</v>
+        <v>13365.65822607783</v>
       </c>
       <c r="V2" t="n">
-        <v>13591.93907272849</v>
+        <v>13555.04381159758</v>
       </c>
       <c r="W2" t="n">
-        <v>13464.51811910982</v>
+        <v>13393.90811692671</v>
       </c>
       <c r="X2" t="n">
-        <v>14438.57227192683</v>
+        <v>14371.5066580513</v>
       </c>
       <c r="Y2" t="n">
-        <v>12327.47698560713</v>
+        <v>12269.54768857951</v>
       </c>
       <c r="Z2" t="n">
-        <v>12631.15330818002</v>
+        <v>12573.78888211672</v>
       </c>
       <c r="AA2" t="n">
-        <v>12648.3146197013</v>
+        <v>12601.14240738908</v>
       </c>
       <c r="AB2" t="n">
-        <v>12076.27218000469</v>
+        <v>12046.89464826908</v>
       </c>
       <c r="AC2" t="n">
-        <v>13074.67615907047</v>
+        <v>13034.55511442974</v>
       </c>
       <c r="AD2" t="n">
-        <v>17435.14891313097</v>
+        <v>17146.73868892287</v>
       </c>
       <c r="AE2" t="n">
-        <v>17720.90628465055</v>
+        <v>17429.79827673879</v>
       </c>
       <c r="AF2" t="n">
-        <v>18746.76134442936</v>
+        <v>18462.52563345131</v>
       </c>
       <c r="AG2" t="n">
-        <v>18819.89780253941</v>
+        <v>18534.4105219489</v>
       </c>
       <c r="AH2" t="n">
-        <v>18735.35924273444</v>
+        <v>18450.41289379931</v>
       </c>
       <c r="AI2" t="n">
-        <v>13860.00612924806</v>
+        <v>16511.20825417279</v>
       </c>
       <c r="AJ2" t="n">
-        <v>12832.05344788632</v>
+        <v>15532.84236131705</v>
       </c>
       <c r="AK2" t="n">
-        <v>13000.71799097621</v>
+        <v>15752.67831301219</v>
+      </c>
+      <c r="AL2" t="n">
+        <v>15445.74022470527</v>
       </c>
     </row>
     <row r="3">
@@ -828,112 +831,115 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>16317.09847029511</v>
+        <v>16317.09863476894</v>
       </c>
       <c r="C3" t="n">
-        <v>15560.49505791214</v>
+        <v>15560.49520672315</v>
       </c>
       <c r="D3" t="n">
-        <v>15140.65068019954</v>
+        <v>15140.65082614158</v>
       </c>
       <c r="E3" t="n">
-        <v>14984.21287200136</v>
+        <v>14984.2130086687</v>
       </c>
       <c r="F3" t="n">
-        <v>14705.10550981868</v>
+        <v>14705.10563862375</v>
       </c>
       <c r="G3" t="n">
-        <v>13791.69661805285</v>
+        <v>13791.69673017739</v>
       </c>
       <c r="H3" t="n">
-        <v>13704.82720745935</v>
+        <v>13704.82208580816</v>
       </c>
       <c r="I3" t="n">
-        <v>14243.18268150757</v>
+        <v>14248.21122685838</v>
       </c>
       <c r="J3" t="n">
-        <v>14459.45299048117</v>
+        <v>14459.45599494156</v>
       </c>
       <c r="K3" t="n">
-        <v>15230.10880037826</v>
+        <v>15230.12185378158</v>
       </c>
       <c r="L3" t="n">
-        <v>15883.25221963124</v>
+        <v>15883.27744660819</v>
       </c>
       <c r="M3" t="n">
-        <v>16391.84139247148</v>
+        <v>16391.87022152429</v>
       </c>
       <c r="N3" t="n">
-        <v>15935.30876474388</v>
+        <v>15935.332424417</v>
       </c>
       <c r="O3" t="n">
-        <v>15256.02663875502</v>
+        <v>15256.06314247587</v>
       </c>
       <c r="P3" t="n">
-        <v>14873.70653373447</v>
+        <v>14873.74447267687</v>
       </c>
       <c r="Q3" t="n">
-        <v>16097.04598985951</v>
+        <v>16097.09173702464</v>
       </c>
       <c r="R3" t="n">
-        <v>16314.89642738784</v>
+        <v>16314.90290949475</v>
       </c>
       <c r="S3" t="n">
-        <v>15996.06426015292</v>
+        <v>15996.07160234409</v>
       </c>
       <c r="T3" t="n">
-        <v>16394.8179629632</v>
+        <v>16394.82749334896</v>
       </c>
       <c r="U3" t="n">
-        <v>16600.63061346446</v>
+        <v>16603.90955716646</v>
       </c>
       <c r="V3" t="n">
-        <v>16787.29240727786</v>
+        <v>16786.9716414575</v>
       </c>
       <c r="W3" t="n">
-        <v>16963.48765639976</v>
+        <v>16963.62551782961</v>
       </c>
       <c r="X3" t="n">
-        <v>17966.42031976848</v>
+        <v>17966.42598843523</v>
       </c>
       <c r="Y3" t="n">
-        <v>16180.31467916186</v>
+        <v>16180.3177144256</v>
       </c>
       <c r="Z3" t="n">
-        <v>16454.10491544267</v>
+        <v>16454.10728186464</v>
       </c>
       <c r="AA3" t="n">
-        <v>16372.48382412917</v>
+        <v>16374.87530200007</v>
       </c>
       <c r="AB3" t="n">
-        <v>15745.91005828504</v>
+        <v>15749.10748630228</v>
       </c>
       <c r="AC3" t="n">
-        <v>15015.12148018784</v>
+        <v>15017.75467608056</v>
       </c>
       <c r="AD3" t="n">
-        <v>13308.0112591078</v>
+        <v>13310.03341191871</v>
       </c>
       <c r="AE3" t="n">
-        <v>13462.60437185618</v>
+        <v>13462.25874068615</v>
       </c>
       <c r="AF3" t="n">
-        <v>14315.70367275086</v>
+        <v>14314.53547147829</v>
       </c>
       <c r="AG3" t="n">
-        <v>14386.52605369849</v>
+        <v>14383.59899219376</v>
       </c>
       <c r="AH3" t="n">
-        <v>14222.8541382654</v>
+        <v>14218.56011470359</v>
       </c>
       <c r="AI3" t="n">
-        <v>13718.38426920016</v>
+        <v>13713.91954691208</v>
       </c>
       <c r="AJ3" t="n">
-        <v>12561.8295122346</v>
+        <v>12562.64245813069</v>
       </c>
       <c r="AK3" t="n">
-        <v>12753.10082184994</v>
+        <v>12753.56238650723</v>
+      </c>
+      <c r="AL3" t="n">
+        <v>12389.63447588753</v>
       </c>
     </row>
     <row r="4">
@@ -943,112 +949,115 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>15667.77876551993</v>
+        <v>15667.77892999376</v>
       </c>
       <c r="C4" t="n">
-        <v>14940.3217041132</v>
+        <v>14940.32185292421</v>
       </c>
       <c r="D4" t="n">
-        <v>14511.19912082284</v>
+        <v>14511.19926676488</v>
       </c>
       <c r="E4" t="n">
-        <v>14355.34507829795</v>
+        <v>14355.34521496529</v>
       </c>
       <c r="F4" t="n">
-        <v>14144.16056780433</v>
+        <v>14144.1606966094</v>
       </c>
       <c r="G4" t="n">
-        <v>13269.48782229216</v>
+        <v>13269.4879344167</v>
       </c>
       <c r="H4" t="n">
-        <v>13133.3111035669</v>
+        <v>13133.30598191571</v>
       </c>
       <c r="I4" t="n">
-        <v>13718.77029143676</v>
+        <v>13723.79883678758</v>
       </c>
       <c r="J4" t="n">
-        <v>13955.96833035105</v>
+        <v>13955.97133481144</v>
       </c>
       <c r="K4" t="n">
-        <v>14698.51427788813</v>
+        <v>14698.52733129145</v>
       </c>
       <c r="L4" t="n">
-        <v>15371.34041593813</v>
+        <v>15371.36564291508</v>
       </c>
       <c r="M4" t="n">
-        <v>15844.02310640728</v>
+        <v>15844.05193546009</v>
       </c>
       <c r="N4" t="n">
-        <v>15390.38651395648</v>
+        <v>15390.4101736296</v>
       </c>
       <c r="O4" t="n">
-        <v>14735.01941846004</v>
+        <v>14735.0559221809</v>
       </c>
       <c r="P4" t="n">
-        <v>14358.87235993313</v>
+        <v>14358.91029887553</v>
       </c>
       <c r="Q4" t="n">
-        <v>15590.68018037227</v>
+        <v>15590.7259275374</v>
       </c>
       <c r="R4" t="n">
-        <v>15760.93570526621</v>
+        <v>15760.94218737313</v>
       </c>
       <c r="S4" t="n">
-        <v>15412.01694540406</v>
+        <v>15412.02428759523</v>
       </c>
       <c r="T4" t="n">
-        <v>15810.88472935007</v>
+        <v>15810.89425973584</v>
       </c>
       <c r="U4" t="n">
-        <v>16031.03108593394</v>
+        <v>16034.31002963594</v>
       </c>
       <c r="V4" t="n">
-        <v>16206.81733769212</v>
+        <v>16206.49657187176</v>
       </c>
       <c r="W4" t="n">
-        <v>16375.5992493916</v>
+        <v>16375.73711082145</v>
       </c>
       <c r="X4" t="n">
-        <v>17396.69626195134</v>
+        <v>17396.70193061809</v>
       </c>
       <c r="Y4" t="n">
-        <v>15619.51336168465</v>
+        <v>15619.51639694839</v>
       </c>
       <c r="Z4" t="n">
-        <v>15890.6142017832</v>
+        <v>15890.61656820517</v>
       </c>
       <c r="AA4" t="n">
-        <v>15799.70625665967</v>
+        <v>15802.09773453056</v>
       </c>
       <c r="AB4" t="n">
-        <v>15188.98040345491</v>
+        <v>15192.17783147215</v>
       </c>
       <c r="AC4" t="n">
-        <v>14519.75592421516</v>
+        <v>14522.38912010788</v>
       </c>
       <c r="AD4" t="n">
-        <v>12919.24115178015</v>
+        <v>12921.26330459106</v>
       </c>
       <c r="AE4" t="n">
-        <v>13061.76216627138</v>
+        <v>13061.41653510135</v>
       </c>
       <c r="AF4" t="n">
-        <v>13886.55825795813</v>
+        <v>13885.39005668556</v>
       </c>
       <c r="AG4" t="n">
-        <v>13945.79136672825</v>
+        <v>13942.86430522352</v>
       </c>
       <c r="AH4" t="n">
-        <v>13802.09145751389</v>
+        <v>13797.79743395207</v>
       </c>
       <c r="AI4" t="n">
-        <v>13309.56839423166</v>
+        <v>13305.10367194358</v>
       </c>
       <c r="AJ4" t="n">
-        <v>12150.51085676689</v>
+        <v>12151.32380266298</v>
       </c>
       <c r="AK4" t="n">
-        <v>12394.40736751538</v>
+        <v>12394.86893217267</v>
+      </c>
+      <c r="AL4" t="n">
+        <v>12081.32220561638</v>
       </c>
     </row>
     <row r="5">
@@ -1118,25 +1127,25 @@
         <v>6449.283897733463</v>
       </c>
       <c r="V5" t="n">
-        <v>6505.65364948456</v>
+        <v>6505.651750900774</v>
       </c>
       <c r="W5" t="n">
-        <v>6726.898652059666</v>
+        <v>6726.898637136408</v>
       </c>
       <c r="X5" t="n">
-        <v>6500.178375851677</v>
+        <v>6500.178422903335</v>
       </c>
       <c r="Y5" t="n">
-        <v>6216.703164691428</v>
+        <v>6216.703164691429</v>
       </c>
       <c r="Z5" t="n">
-        <v>6346.730894556922</v>
+        <v>6346.730894556923</v>
       </c>
       <c r="AA5" t="n">
         <v>6366.053448168976</v>
       </c>
       <c r="AB5" t="n">
-        <v>6058.818071311212</v>
+        <v>6058.81807131121</v>
       </c>
       <c r="AC5" t="n">
         <v>5778.78136425101</v>
@@ -1164,6 +1173,9 @@
       </c>
       <c r="AK5" t="n">
         <v>4198.372080304202</v>
+      </c>
+      <c r="AL5" t="n">
+        <v>3415.580184169819</v>
       </c>
     </row>
     <row r="6">
@@ -1194,7 +1206,7 @@
         <v>2585.674246989111</v>
       </c>
       <c r="I6" t="n">
-        <v>2512.636429858072</v>
+        <v>2517.66998620219</v>
       </c>
       <c r="J6" t="n">
         <v>2681.000912985214</v>
@@ -1206,7 +1218,7 @@
         <v>2521.369797655697</v>
       </c>
       <c r="M6" t="n">
-        <v>2300.399657864836</v>
+        <v>2300.399657864835</v>
       </c>
       <c r="N6" t="n">
         <v>2281.479258241734</v>
@@ -1218,7 +1230,7 @@
         <v>2293.438728812481</v>
       </c>
       <c r="Q6" t="n">
-        <v>2212.708519097478</v>
+        <v>2212.708519097479</v>
       </c>
       <c r="R6" t="n">
         <v>2244.527626783632</v>
@@ -1230,22 +1242,22 @@
         <v>2325.438090669641</v>
       </c>
       <c r="U6" t="n">
-        <v>2461.103479663697</v>
+        <v>2464.132211434577</v>
       </c>
       <c r="V6" t="n">
         <v>2599.94864496337</v>
       </c>
       <c r="W6" t="n">
-        <v>2362.814375535351</v>
+        <v>2362.834981158305</v>
       </c>
       <c r="X6" t="n">
         <v>2334.85686114773</v>
       </c>
       <c r="Y6" t="n">
-        <v>1957.241684003474</v>
+        <v>1957.242626213672</v>
       </c>
       <c r="Z6" t="n">
-        <v>1932.303533129637</v>
+        <v>1932.304141867118</v>
       </c>
       <c r="AA6" t="n">
         <v>1732.01861936165</v>
@@ -1279,6 +1291,9 @@
       </c>
       <c r="AK6" t="n">
         <v>1732.555035058429</v>
+      </c>
+      <c r="AL6" t="n">
+        <v>1605.367235979008</v>
       </c>
     </row>
     <row r="7">
@@ -1288,112 +1303,115 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>2051.166581011497</v>
+        <v>2051.166745485325</v>
       </c>
       <c r="C7" t="n">
-        <v>2424.905568512975</v>
+        <v>2424.905717323991</v>
       </c>
       <c r="D7" t="n">
-        <v>2454.530366495709</v>
+        <v>2454.530512437749</v>
       </c>
       <c r="E7" t="n">
-        <v>2484.697846971827</v>
+        <v>2484.697983639161</v>
       </c>
       <c r="F7" t="n">
-        <v>2737.214541860846</v>
+        <v>2737.214670665915</v>
       </c>
       <c r="G7" t="n">
-        <v>2593.352835041149</v>
+        <v>2593.352947165686</v>
       </c>
       <c r="H7" t="n">
-        <v>2635.30849325366</v>
+        <v>2635.303371602473</v>
       </c>
       <c r="I7" t="n">
-        <v>3185.127453689799</v>
+        <v>3185.122442696496</v>
       </c>
       <c r="J7" t="n">
-        <v>3569.719543035433</v>
+        <v>3569.722547495825</v>
       </c>
       <c r="K7" t="n">
-        <v>3988.888799732674</v>
+        <v>3988.901853135989</v>
       </c>
       <c r="L7" t="n">
-        <v>4530.06041075233</v>
+        <v>4530.085637729284</v>
       </c>
       <c r="M7" t="n">
-        <v>4737.73791826305</v>
+        <v>4737.766747315859</v>
       </c>
       <c r="N7" t="n">
-        <v>3939.897236794766</v>
+        <v>3939.920896467887</v>
       </c>
       <c r="O7" t="n">
-        <v>3729.689672076353</v>
+        <v>3729.726175797206</v>
       </c>
       <c r="P7" t="n">
-        <v>3676.079143435267</v>
+        <v>3676.117082377669</v>
       </c>
       <c r="Q7" t="n">
-        <v>3837.127046627688</v>
+        <v>3837.172793792819</v>
       </c>
       <c r="R7" t="n">
-        <v>3904.168352321483</v>
+        <v>3904.1748344284</v>
       </c>
       <c r="S7" t="n">
-        <v>3953.666424596537</v>
+        <v>3953.673766787709</v>
       </c>
       <c r="T7" t="n">
-        <v>4132.137211291438</v>
+        <v>4132.144391467687</v>
       </c>
       <c r="U7" t="n">
-        <v>4401.338486719485</v>
+        <v>4401.345895475234</v>
       </c>
       <c r="V7" t="n">
-        <v>4637.346939012829</v>
+        <v>4637.354031608292</v>
       </c>
       <c r="W7" t="n">
-        <v>5239.947181615161</v>
+        <v>5239.952781905618</v>
       </c>
       <c r="X7" t="n">
-        <v>6159.07967847829</v>
+        <v>6159.085300093378</v>
       </c>
       <c r="Y7" t="n">
-        <v>5158.764432965329</v>
+        <v>5158.766527499439</v>
       </c>
       <c r="Z7" t="n">
-        <v>5299.219368482122</v>
+        <v>5299.221126544413</v>
       </c>
       <c r="AA7" t="n">
-        <v>5649.476969390869</v>
+        <v>5649.478548164547</v>
       </c>
       <c r="AB7" t="n">
-        <v>5668.060125583393</v>
+        <v>5668.09462407233</v>
       </c>
       <c r="AC7" t="n">
-        <v>5367.270528846784</v>
+        <v>5367.304329827344</v>
       </c>
       <c r="AD7" t="n">
-        <v>5383.263647751578</v>
+        <v>5383.31201974678</v>
       </c>
       <c r="AE7" t="n">
-        <v>5353.648884363555</v>
+        <v>5353.747959454742</v>
       </c>
       <c r="AF7" t="n">
-        <v>5726.818184752282</v>
+        <v>5726.945141299557</v>
       </c>
       <c r="AG7" t="n">
-        <v>5856.284530716071</v>
+        <v>5856.458601399291</v>
       </c>
       <c r="AH7" t="n">
-        <v>5835.006116667818</v>
+        <v>5835.176020166483</v>
       </c>
       <c r="AI7" t="n">
-        <v>5624.997279783624</v>
+        <v>5625.18568894176</v>
       </c>
       <c r="AJ7" t="n">
-        <v>4575.48795380118</v>
+        <v>4575.713557529093</v>
       </c>
       <c r="AK7" t="n">
-        <v>5205.456914637582</v>
+        <v>5205.492546308518</v>
+      </c>
+      <c r="AL7" t="n">
+        <v>5794.232273170996</v>
       </c>
     </row>
     <row r="8">
@@ -1403,7 +1421,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>2611.850486393283</v>
+        <v>2611.850486393282</v>
       </c>
       <c r="C8" t="n">
         <v>2321.062169688189</v>
@@ -1412,16 +1430,16 @@
         <v>1921.097400043078</v>
       </c>
       <c r="E8" t="n">
-        <v>1838.837337070248</v>
+        <v>1838.837337070249</v>
       </c>
       <c r="F8" t="n">
         <v>1905.615208824076</v>
       </c>
       <c r="G8" t="n">
-        <v>2162.97515218897</v>
+        <v>2162.975152188971</v>
       </c>
       <c r="H8" t="n">
-        <v>1947.811368801155</v>
+        <v>1947.811368801154</v>
       </c>
       <c r="I8" t="n">
         <v>2266.365925006984</v>
@@ -1442,31 +1460,31 @@
         <v>3180.246369034387</v>
       </c>
       <c r="O8" t="n">
-        <v>3418.631256553266</v>
+        <v>3418.631256553267</v>
       </c>
       <c r="P8" t="n">
         <v>2793.322667610508</v>
       </c>
       <c r="Q8" t="n">
-        <v>3227.039105441017</v>
+        <v>3227.039105441018</v>
       </c>
       <c r="R8" t="n">
-        <v>3045.774890649536</v>
+        <v>3045.774890649537</v>
       </c>
       <c r="S8" t="n">
         <v>2990.171721181347</v>
       </c>
       <c r="T8" t="n">
-        <v>2927.65133187209</v>
+        <v>2927.653682081602</v>
       </c>
       <c r="U8" t="n">
-        <v>2715.980218311699</v>
+        <v>2716.223021487069</v>
       </c>
       <c r="V8" t="n">
-        <v>2460.543100725764</v>
+        <v>2460.217140893727</v>
       </c>
       <c r="W8" t="n">
-        <v>2042.457196887822</v>
+        <v>2042.568867327516</v>
       </c>
       <c r="X8" t="n">
         <v>2399.028897044284</v>
@@ -1475,40 +1493,43 @@
         <v>2283.465558585317</v>
       </c>
       <c r="Z8" t="n">
-        <v>2309.472078205791</v>
+        <v>2309.472078205665</v>
       </c>
       <c r="AA8" t="n">
-        <v>2048.789037121608</v>
+        <v>2051.178937336148</v>
       </c>
       <c r="AB8" t="n">
-        <v>1796.190680255663</v>
+        <v>1799.353608378683</v>
       </c>
       <c r="AC8" t="n">
-        <v>1715.105023322609</v>
+        <v>1717.704419474934</v>
       </c>
       <c r="AD8" t="n">
-        <v>1417.577336925175</v>
+        <v>1419.551118109141</v>
       </c>
       <c r="AE8" t="n">
-        <v>1533.933800551959</v>
+        <v>1533.48909429074</v>
       </c>
       <c r="AF8" t="n">
-        <v>1603.582264770285</v>
+        <v>1602.287106950443</v>
       </c>
       <c r="AG8" t="n">
-        <v>1471.291666502438</v>
+        <v>1468.190534314485</v>
       </c>
       <c r="AH8" t="n">
-        <v>1367.128948419185</v>
+        <v>1362.665021358706</v>
       </c>
       <c r="AI8" t="n">
-        <v>1353.72015242035</v>
+        <v>1349.067020974135</v>
       </c>
       <c r="AJ8" t="n">
-        <v>1354.434757284797</v>
+        <v>1355.022099452973</v>
       </c>
       <c r="AK8" t="n">
-        <v>1253.433044703854</v>
+        <v>1253.858977690213</v>
+      </c>
+      <c r="AL8" t="n">
+        <v>1261.456139431114</v>
       </c>
     </row>
     <row r="9">
@@ -1518,7 +1539,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>41.405704032</v>
+        <v>41.40570403199999</v>
       </c>
       <c r="C9" t="n">
         <v>31.995316752</v>
@@ -1587,22 +1608,22 @@
         <v>3.55244942936184</v>
       </c>
       <c r="Y9" t="n">
-        <v>3.3385214390971</v>
+        <v>3.33851995852984</v>
       </c>
       <c r="Z9" t="n">
-        <v>2.88832740872364</v>
+        <v>2.88832703105464</v>
       </c>
       <c r="AA9" t="n">
-        <v>3.36818261656348</v>
+        <v>3.3681814992364</v>
       </c>
       <c r="AB9" t="n">
-        <v>3.37640163563943</v>
+        <v>3.37640304092336</v>
       </c>
       <c r="AC9" t="n">
-        <v>3.01296571394668</v>
+        <v>3.01296447378248</v>
       </c>
       <c r="AD9" t="n">
-        <v>3.75059177539285</v>
+        <v>3.75059140713376</v>
       </c>
       <c r="AE9" t="n">
         <v>3.69786187040816</v>
@@ -1624,6 +1645,9 @@
       </c>
       <c r="AK9" t="n">
         <v>4.5902928113112</v>
+      </c>
+      <c r="AL9" t="n">
+        <v>4.68637286544</v>
       </c>
     </row>
     <row r="10">
@@ -1740,6 +1764,9 @@
       <c r="AK10" t="n">
         <v>358.6934543345557</v>
       </c>
+      <c r="AL10" t="n">
+        <v>308.312270271158</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="4" t="inlineStr">
@@ -1855,6 +1882,9 @@
       <c r="AK11" t="n">
         <v>312.6453405780825</v>
       </c>
+      <c r="AL11" t="n">
+        <v>267.3401138417487</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="4" t="inlineStr">
@@ -1970,6 +2000,9 @@
       <c r="AK12" t="n">
         <v>46.0481137564731</v>
       </c>
+      <c r="AL12" t="n">
+        <v>40.97215642940919</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="4" t="inlineStr">
@@ -1985,112 +2018,115 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>1585.886765890986</v>
+        <v>1585.933758473278</v>
       </c>
       <c r="C14" t="n">
-        <v>1566.629765801041</v>
+        <v>1566.676758795625</v>
       </c>
       <c r="D14" t="n">
-        <v>1465.403879320702</v>
+        <v>1465.450872306664</v>
       </c>
       <c r="E14" t="n">
-        <v>1410.635365295763</v>
+        <v>1410.682358433192</v>
       </c>
       <c r="F14" t="n">
-        <v>1367.876281450622</v>
+        <v>1367.946774505304</v>
       </c>
       <c r="G14" t="n">
-        <v>1057.017948715313</v>
+        <v>1057.088442372029</v>
       </c>
       <c r="H14" t="n">
-        <v>1047.321269566099</v>
+        <v>1047.392027769271</v>
       </c>
       <c r="I14" t="n">
-        <v>874.6386137857995</v>
+        <v>874.7093920685608</v>
       </c>
       <c r="J14" t="n">
-        <v>1051.184816781642</v>
+        <v>1051.255453222576</v>
       </c>
       <c r="K14" t="n">
-        <v>1056.358239910607</v>
+        <v>1056.452558740726</v>
       </c>
       <c r="L14" t="n">
-        <v>1057.842461433635</v>
+        <v>1057.936738644809</v>
       </c>
       <c r="M14" t="n">
-        <v>1097.038283898761</v>
+        <v>1098.307760373769</v>
       </c>
       <c r="N14" t="n">
-        <v>1075.211025392189</v>
+        <v>1075.412925243019</v>
       </c>
       <c r="O14" t="n">
-        <v>1099.291150344979</v>
+        <v>1099.492828338277</v>
       </c>
       <c r="P14" t="n">
-        <v>1141.123584393479</v>
+        <v>1141.325026635718</v>
       </c>
       <c r="Q14" t="n">
-        <v>1196.90447492802</v>
+        <v>1197.129300843065</v>
       </c>
       <c r="R14" t="n">
-        <v>1203.843425031441</v>
+        <v>1204.0800544709</v>
       </c>
       <c r="S14" t="n">
-        <v>1271.402730195529</v>
+        <v>1271.639362508384</v>
       </c>
       <c r="T14" t="n">
-        <v>1321.818673246448</v>
+        <v>1322.055307416907</v>
       </c>
       <c r="U14" t="n">
-        <v>1394.631564356943</v>
+        <v>1394.868197189202</v>
       </c>
       <c r="V14" t="n">
-        <v>1438.83624719657</v>
+        <v>1439.096380611895</v>
       </c>
       <c r="W14" t="n">
-        <v>1448.780540918582</v>
+        <v>1449.046783233174</v>
       </c>
       <c r="X14" t="n">
-        <v>1322.27263132632</v>
+        <v>1322.538873165317</v>
       </c>
       <c r="Y14" t="n">
-        <v>985.6141215127182</v>
+        <v>985.9099732261653</v>
       </c>
       <c r="Z14" t="n">
-        <v>986.4021232488136</v>
+        <v>986.7214759540102</v>
       </c>
       <c r="AA14" t="n">
-        <v>997.3635058547696</v>
+        <v>998.8639689732466</v>
       </c>
       <c r="AB14" t="n">
-        <v>1023.624822002169</v>
+        <v>1023.95028585115</v>
       </c>
       <c r="AC14" t="n">
-        <v>1090.763229655807</v>
+        <v>1091.095493800481</v>
       </c>
       <c r="AD14" t="n">
-        <v>1127.971091877877</v>
+        <v>1128.304345723169</v>
       </c>
       <c r="AE14" t="n">
-        <v>1107.87076432244</v>
+        <v>1108.798090535365</v>
       </c>
       <c r="AF14" t="n">
-        <v>1114.398729489344</v>
+        <v>1114.739383410253</v>
       </c>
       <c r="AG14" t="n">
-        <v>1171.848866051391</v>
+        <v>1173.263768751868</v>
       </c>
       <c r="AH14" t="n">
-        <v>1195.046308572837</v>
+        <v>1196.249945662347</v>
       </c>
       <c r="AI14" t="n">
-        <v>1204.549735246576</v>
+        <v>1206.189335265369</v>
       </c>
       <c r="AJ14" t="n">
-        <v>1148.841530201404</v>
+        <v>1153.64766774399</v>
       </c>
       <c r="AK14" t="n">
-        <v>1111.135487745607</v>
+        <v>1127.447356606783</v>
+      </c>
+      <c r="AL14" t="n">
+        <v>1138.911884394025</v>
       </c>
     </row>
     <row r="15">
@@ -2207,6 +2243,9 @@
       <c r="AK15" t="n">
         <v>567.526706760132</v>
       </c>
+      <c r="AL15" t="n">
+        <v>574.1230258072445</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="4" t="inlineStr">
@@ -2322,6 +2361,9 @@
       <c r="AK16" t="n">
         <v>65.212739461791</v>
       </c>
+      <c r="AL16" t="n">
+        <v>64.80501058608465</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="4" t="inlineStr">
@@ -2437,6 +2479,9 @@
       <c r="AK17" t="n">
         <v>129.0734739323934</v>
       </c>
+      <c r="AL17" t="n">
+        <v>89.33613529026272</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="5" t="inlineStr">
@@ -2445,112 +2490,115 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>8.13615300911459</v>
+        <v>8.13614559140605</v>
       </c>
       <c r="C18" t="n">
-        <v>8.55056331579576</v>
+        <v>8.55055631038023</v>
       </c>
       <c r="D18" t="n">
-        <v>8.90845134246004</v>
+        <v>8.90844432842184</v>
       </c>
       <c r="E18" t="n">
-        <v>9.147520017598129</v>
+        <v>9.1475131550276</v>
       </c>
       <c r="F18" t="n">
-        <v>8.496062234601389</v>
+        <v>8.496055289283071</v>
       </c>
       <c r="G18" t="n">
-        <v>8.421207431252331</v>
+        <v>8.421201087968161</v>
       </c>
       <c r="H18" t="n">
-        <v>7.35853697149717</v>
+        <v>7.35879517466904</v>
       </c>
       <c r="I18" t="n">
-        <v>8.30925574944852</v>
+        <v>8.309534032209751</v>
       </c>
       <c r="J18" t="n">
-        <v>8.34152936331872</v>
+        <v>8.341665804252781</v>
       </c>
       <c r="K18" t="n">
-        <v>6.71758445220387</v>
+        <v>6.71790328232305</v>
       </c>
       <c r="L18" t="n">
-        <v>8.33220722306584</v>
+        <v>8.33248443424031</v>
       </c>
       <c r="M18" t="n">
-        <v>12.67127256794094</v>
+        <v>12.67174904294875</v>
       </c>
       <c r="N18" t="n">
-        <v>16.82193957078551</v>
+        <v>16.82291442161512</v>
       </c>
       <c r="O18" t="n">
-        <v>15.22350778108833</v>
+        <v>15.22426077438689</v>
       </c>
       <c r="P18" t="n">
-        <v>14.1406786601579</v>
+        <v>14.14119590239678</v>
       </c>
       <c r="Q18" t="n">
-        <v>23.2363864554548</v>
+        <v>23.23678737050032</v>
       </c>
       <c r="R18" t="n">
-        <v>23.75329114108768</v>
+        <v>23.75327558054685</v>
       </c>
       <c r="S18" t="n">
-        <v>18.70445427664346</v>
+        <v>18.70444158949923</v>
       </c>
       <c r="T18" t="n">
-        <v>27.83241546433778</v>
+        <v>27.83240463479622</v>
       </c>
       <c r="U18" t="n">
-        <v>24.91009368106351</v>
+        <v>24.91008151332242</v>
       </c>
       <c r="V18" t="n">
-        <v>26.48638948983933</v>
+        <v>26.48637790516396</v>
       </c>
       <c r="W18" t="n">
-        <v>22.19730362492648</v>
+        <v>22.19729093951875</v>
       </c>
       <c r="X18" t="n">
-        <v>19.75285695500772</v>
+        <v>19.75284379400384</v>
       </c>
       <c r="Y18" t="n">
-        <v>17.12706282444312</v>
+        <v>17.12704953789023</v>
       </c>
       <c r="Z18" t="n">
-        <v>14.8134239929981</v>
+        <v>14.81341169819465</v>
       </c>
       <c r="AA18" t="n">
-        <v>16.68203320082564</v>
+        <v>16.68202131930267</v>
       </c>
       <c r="AB18" t="n">
-        <v>20.41502833904076</v>
+        <v>20.41501718802209</v>
       </c>
       <c r="AC18" t="n">
-        <v>17.84788128883862</v>
+        <v>17.84856043351264</v>
       </c>
       <c r="AD18" t="n">
-        <v>23.58723041658946</v>
+        <v>23.58889926188098</v>
       </c>
       <c r="AE18" t="n">
-        <v>25.64876666288793</v>
+        <v>25.65089787581219</v>
       </c>
       <c r="AF18" t="n">
-        <v>26.16209920369645</v>
+        <v>26.16505812460512</v>
       </c>
       <c r="AG18" t="n">
-        <v>31.31585052246558</v>
+        <v>31.32944822294178</v>
       </c>
       <c r="AH18" t="n">
-        <v>33.76744203953536</v>
+        <v>33.78127412904553</v>
       </c>
       <c r="AI18" t="n">
-        <v>32.75603630958375</v>
+        <v>32.75755838342308</v>
       </c>
       <c r="AJ18" t="n">
-        <v>31.0116462229686</v>
+        <v>31.01283590157006</v>
       </c>
       <c r="AK18" t="n">
-        <v>34.60032849097653</v>
+        <v>34.59982019382382</v>
+      </c>
+      <c r="AL18" t="n">
+        <v>14.98857247025259</v>
       </c>
     </row>
     <row r="19">
@@ -2645,13 +2693,16 @@
         <v>304.6051014962227</v>
       </c>
       <c r="AI20" t="n">
-        <v>282.1905939552199</v>
+        <v>282.756366900173</v>
       </c>
       <c r="AJ20" t="n">
-        <v>277.7612655111739</v>
+        <v>281.387218375159</v>
       </c>
       <c r="AK20" t="n">
-        <v>267.039430544354</v>
+        <v>282.924812702683</v>
+      </c>
+      <c r="AL20" t="n">
+        <v>281.8648534436099</v>
       </c>
     </row>
     <row r="21">
@@ -2661,112 +2712,115 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>80.08381</v>
+        <v>80.13081</v>
       </c>
       <c r="C21" t="n">
-        <v>71.855295</v>
+        <v>71.902295</v>
       </c>
       <c r="D21" t="n">
-        <v>63.62678</v>
+        <v>63.67378</v>
       </c>
       <c r="E21" t="n">
-        <v>56.601465</v>
+        <v>56.648465</v>
       </c>
       <c r="F21" t="n">
-        <v>47.23085</v>
+        <v>47.30135</v>
       </c>
       <c r="G21" t="n">
-        <v>41.7405</v>
+        <v>41.811</v>
       </c>
       <c r="H21" t="n">
-        <v>33.814</v>
+        <v>33.8845</v>
       </c>
       <c r="I21" t="n">
-        <v>27.688635</v>
+        <v>27.759135</v>
       </c>
       <c r="J21" t="n">
-        <v>27.27042</v>
+        <v>27.34092</v>
       </c>
       <c r="K21" t="n">
-        <v>27.25107</v>
+        <v>27.34507</v>
       </c>
       <c r="L21" t="n">
-        <v>29.2576</v>
+        <v>29.3516</v>
       </c>
       <c r="M21" t="n">
-        <v>29.85735</v>
+        <v>31.12635</v>
       </c>
       <c r="N21" t="n">
-        <v>37.060315</v>
+        <v>37.26124</v>
       </c>
       <c r="O21" t="n">
-        <v>43.536305</v>
+        <v>43.73723</v>
       </c>
       <c r="P21" t="n">
-        <v>52.00076</v>
+        <v>52.201685</v>
       </c>
       <c r="Q21" t="n">
-        <v>46.92774</v>
+        <v>47.152165</v>
       </c>
       <c r="R21" t="n">
-        <v>48.273475</v>
+        <v>48.51012</v>
       </c>
       <c r="S21" t="n">
-        <v>46.109195</v>
+        <v>46.34584</v>
       </c>
       <c r="T21" t="n">
-        <v>51.5547</v>
+        <v>51.791345</v>
       </c>
       <c r="U21" t="n">
-        <v>55.580838625</v>
+        <v>55.817483625</v>
       </c>
       <c r="V21" t="n">
-        <v>56.227894265265</v>
+        <v>56.488039265265</v>
       </c>
       <c r="W21" t="n">
-        <v>54.08715505421</v>
+        <v>54.35341005421</v>
       </c>
       <c r="X21" t="n">
-        <v>43.55024168751</v>
+        <v>43.81649668751</v>
       </c>
       <c r="Y21" t="n">
-        <v>44.19195385</v>
+        <v>44.48781885</v>
       </c>
       <c r="Z21" t="n">
-        <v>43.678334525</v>
+        <v>43.997699525</v>
       </c>
       <c r="AA21" t="n">
-        <v>60.013065625</v>
+        <v>61.513540625</v>
       </c>
       <c r="AB21" t="n">
-        <v>67.96800462500001</v>
+        <v>68.293479625</v>
       </c>
       <c r="AC21" t="n">
-        <v>48.655093</v>
+        <v>48.986678</v>
       </c>
       <c r="AD21" t="n">
-        <v>38.077597775</v>
+        <v>38.409182775</v>
       </c>
       <c r="AE21" t="n">
-        <v>50.98166275</v>
+        <v>51.90685775</v>
       </c>
       <c r="AF21" t="n">
-        <v>50.9220045925</v>
+        <v>51.2596995925</v>
       </c>
       <c r="AG21" t="n">
-        <v>34.408689675</v>
+        <v>35.809994675</v>
       </c>
       <c r="AH21" t="n">
-        <v>41.83276723138</v>
+        <v>43.02257223138</v>
       </c>
       <c r="AI21" t="n">
-        <v>75.2240811905</v>
+        <v>76.2963861905</v>
       </c>
       <c r="AJ21" t="n">
-        <v>75.51054013596</v>
+        <v>76.68953513596</v>
       </c>
       <c r="AK21" t="n">
-        <v>47.68280855596</v>
+        <v>48.10980355596</v>
+      </c>
+      <c r="AL21" t="n">
+        <v>113.79428679657</v>
       </c>
     </row>
     <row r="22">
@@ -2783,112 +2837,115 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>2029.474908792829</v>
+        <v>2038.447456990076</v>
       </c>
       <c r="C23" t="n">
-        <v>2036.878599637079</v>
+        <v>2046.052587222948</v>
       </c>
       <c r="D23" t="n">
-        <v>2001.111173986862</v>
+        <v>2010.049887814222</v>
       </c>
       <c r="E23" t="n">
-        <v>1964.884459198629</v>
+        <v>1973.00837734127</v>
       </c>
       <c r="F23" t="n">
-        <v>1951.30178836969</v>
+        <v>1960.068785847821</v>
       </c>
       <c r="G23" t="n">
-        <v>1832.54016808878</v>
+        <v>1834.792305529219</v>
       </c>
       <c r="H23" t="n">
-        <v>1947.358840788389</v>
+        <v>1954.781140960901</v>
       </c>
       <c r="I23" t="n">
-        <v>1838.742499236762</v>
+        <v>1846.396794055564</v>
       </c>
       <c r="J23" t="n">
-        <v>1855.137138571591</v>
+        <v>1859.429503680643</v>
       </c>
       <c r="K23" t="n">
-        <v>1855.023754577756</v>
+        <v>1856.494582757377</v>
       </c>
       <c r="L23" t="n">
-        <v>1793.791374575547</v>
+        <v>1783.434595119798</v>
       </c>
       <c r="M23" t="n">
-        <v>1743.341407712839</v>
+        <v>1732.607924387543</v>
       </c>
       <c r="N23" t="n">
-        <v>1783.309638316269</v>
+        <v>1770.963497004401</v>
       </c>
       <c r="O23" t="n">
-        <v>1799.007550071298</v>
+        <v>1784.157432316439</v>
       </c>
       <c r="P23" t="n">
-        <v>1892.158924254998</v>
+        <v>1871.157218660298</v>
       </c>
       <c r="Q23" t="n">
-        <v>1867.710264005515</v>
+        <v>1845.226625288445</v>
       </c>
       <c r="R23" t="n">
-        <v>1928.001910383253</v>
+        <v>1900.852660739891</v>
       </c>
       <c r="S23" t="n">
-        <v>1832.83021659404</v>
+        <v>1808.511290997384</v>
       </c>
       <c r="T23" t="n">
-        <v>1781.473809774056</v>
+        <v>1761.618141619746</v>
       </c>
       <c r="U23" t="n">
-        <v>1798.73480161636</v>
+        <v>1769.143133415147</v>
       </c>
       <c r="V23" t="n">
-        <v>1797.92793830388</v>
+        <v>1767.715370379963</v>
       </c>
       <c r="W23" t="n">
-        <v>1858.885665034147</v>
+        <v>1825.113901569189</v>
       </c>
       <c r="X23" t="n">
-        <v>1781.552347895328</v>
+        <v>1748.470642326046</v>
       </c>
       <c r="Y23" t="n">
-        <v>1790.482907875046</v>
+        <v>1758.229839646414</v>
       </c>
       <c r="Z23" t="n">
-        <v>1758.289205766902</v>
+        <v>1726.443890609153</v>
       </c>
       <c r="AA23" t="n">
-        <v>1740.606766527864</v>
+        <v>1708.42639965658</v>
       </c>
       <c r="AB23" t="n">
-        <v>1724.582300183074</v>
+        <v>1692.620869818552</v>
       </c>
       <c r="AC23" t="n">
-        <v>1709.193605615291</v>
+        <v>1678.915596273104</v>
       </c>
       <c r="AD23" t="n">
-        <v>1756.007270328623</v>
+        <v>1721.452283447518</v>
       </c>
       <c r="AE23" t="n">
-        <v>1799.502089434028</v>
+        <v>1763.610101907941</v>
       </c>
       <c r="AF23" t="n">
-        <v>1822.166366175141</v>
+        <v>1782.434835920687</v>
       </c>
       <c r="AG23" t="n">
-        <v>1787.842412683291</v>
+        <v>1749.117983720161</v>
       </c>
       <c r="AH23" t="n">
-        <v>1787.575306141831</v>
+        <v>1748.929298173952</v>
       </c>
       <c r="AI23" t="n">
-        <v>1807.850420765808</v>
+        <v>1768.627419686267</v>
       </c>
       <c r="AJ23" t="n">
-        <v>1812.994330967829</v>
+        <v>1773.361771848206</v>
       </c>
       <c r="AK23" t="n">
-        <v>1813.4704783226</v>
+        <v>1773.733925238289</v>
+      </c>
+      <c r="AL23" t="n">
+        <v>1706.324827020979</v>
       </c>
     </row>
     <row r="24">
@@ -2898,112 +2955,115 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>1098.479069163331</v>
+        <v>1115.649774207144</v>
       </c>
       <c r="C24" t="n">
-        <v>1077.381227426218</v>
+        <v>1094.411722618398</v>
       </c>
       <c r="D24" t="n">
-        <v>1071.364972309792</v>
+        <v>1088.129495036329</v>
       </c>
       <c r="E24" t="n">
-        <v>1067.767794328299</v>
+        <v>1083.65446158653</v>
       </c>
       <c r="F24" t="n">
-        <v>1047.479895771825</v>
+        <v>1063.915991345167</v>
       </c>
       <c r="G24" t="n">
-        <v>991.1658030891829</v>
+        <v>1001.597680341271</v>
       </c>
       <c r="H24" t="n">
-        <v>1005.986245203149</v>
+        <v>1020.858392802735</v>
       </c>
       <c r="I24" t="n">
-        <v>959.8566059149242</v>
+        <v>974.5751055965943</v>
       </c>
       <c r="J24" t="n">
-        <v>968.7229413757949</v>
+        <v>980.3900496806996</v>
       </c>
       <c r="K24" t="n">
-        <v>1012.762791861665</v>
+        <v>1021.990074840394</v>
       </c>
       <c r="L24" t="n">
-        <v>992.299186797452</v>
+        <v>989.2795173858411</v>
       </c>
       <c r="M24" t="n">
-        <v>937.6611746226528</v>
+        <v>934.2058779103202</v>
       </c>
       <c r="N24" t="n">
-        <v>957.0764683532469</v>
+        <v>952.1823326458926</v>
       </c>
       <c r="O24" t="n">
-        <v>998.7479184580455</v>
+        <v>991.7953222858534</v>
       </c>
       <c r="P24" t="n">
-        <v>1062.801536106535</v>
+        <v>1049.890044063107</v>
       </c>
       <c r="Q24" t="n">
-        <v>1043.41742450936</v>
+        <v>1029.091322871097</v>
       </c>
       <c r="R24" t="n">
-        <v>1075.20815820994</v>
+        <v>1057.160932637948</v>
       </c>
       <c r="S24" t="n">
-        <v>1015.57994869473</v>
+        <v>999.5627482335838</v>
       </c>
       <c r="T24" t="n">
-        <v>1007.851851974717</v>
+        <v>994.1237299823987</v>
       </c>
       <c r="U24" t="n">
-        <v>1025.444306054811</v>
+        <v>1004.829314186717</v>
       </c>
       <c r="V24" t="n">
-        <v>1022.047643066487</v>
+        <v>999.1805531522181</v>
       </c>
       <c r="W24" t="n">
-        <v>1066.058606700411</v>
+        <v>1041.90792336144</v>
       </c>
       <c r="X24" t="n">
-        <v>1041.61986969053</v>
+        <v>1017.625544051278</v>
       </c>
       <c r="Y24" t="n">
-        <v>1024.988142341259</v>
+        <v>1003.327438946733</v>
       </c>
       <c r="Z24" t="n">
-        <v>1010.861185424984</v>
+        <v>989.452778205477</v>
       </c>
       <c r="AA24" t="n">
-        <v>1011.126681494633</v>
+        <v>989.5649058436971</v>
       </c>
       <c r="AB24" t="n">
-        <v>1006.884230934852</v>
+        <v>984.9144284935007</v>
       </c>
       <c r="AC24" t="n">
-        <v>995.4461178694195</v>
+        <v>974.8582356819121</v>
       </c>
       <c r="AD24" t="n">
-        <v>1016.959486788103</v>
+        <v>993.484094223738</v>
       </c>
       <c r="AE24" t="n">
-        <v>1047.837127434899</v>
+        <v>1024.612035818532</v>
       </c>
       <c r="AF24" t="n">
-        <v>1065.361946016077</v>
+        <v>1037.970137170018</v>
       </c>
       <c r="AG24" t="n">
-        <v>1043.539531486069</v>
+        <v>1017.383679379229</v>
       </c>
       <c r="AH24" t="n">
-        <v>1038.429303150085</v>
+        <v>1010.879460646789</v>
       </c>
       <c r="AI24" t="n">
-        <v>1051.965475922688</v>
+        <v>1023.485162101747</v>
       </c>
       <c r="AJ24" t="n">
-        <v>1054.643721224549</v>
+        <v>1024.667132737476</v>
       </c>
       <c r="AK24" t="n">
-        <v>1051.472371414404</v>
+        <v>1021.758064833655</v>
+      </c>
+      <c r="AL24" t="n">
+        <v>984.8949985044593</v>
       </c>
     </row>
     <row r="25">
@@ -3013,112 +3073,115 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>449.7136008553759</v>
+        <v>447.5732184902475</v>
       </c>
       <c r="C25" t="n">
-        <v>455.0408344239258</v>
+        <v>452.9897313075099</v>
       </c>
       <c r="D25" t="n">
-        <v>446.772397376849</v>
+        <v>444.7293163988921</v>
       </c>
       <c r="E25" t="n">
-        <v>438.6820361030766</v>
+        <v>436.6554338098041</v>
       </c>
       <c r="F25" t="n">
-        <v>444.8535535059551</v>
+        <v>442.8514239518415</v>
       </c>
       <c r="G25" t="n">
-        <v>417.3661624926438</v>
+        <v>415.2340875436075</v>
       </c>
       <c r="H25" t="n">
-        <v>435.0618160185422</v>
+        <v>433.123323844393</v>
       </c>
       <c r="I25" t="n">
-        <v>413.8785657973725</v>
+        <v>412.0434965693123</v>
       </c>
       <c r="J25" t="n">
-        <v>412.3335805153504</v>
+        <v>410.4208432507924</v>
       </c>
       <c r="K25" t="n">
-        <v>384.166547966283</v>
+        <v>382.1579319731063</v>
       </c>
       <c r="L25" t="n">
-        <v>364.5765263516838</v>
+        <v>362.6794438111023</v>
       </c>
       <c r="M25" t="n">
-        <v>364.6614700262504</v>
+        <v>362.7824277602041</v>
       </c>
       <c r="N25" t="n">
-        <v>372.9234053204821</v>
+        <v>371.0022929480015</v>
       </c>
       <c r="O25" t="n">
-        <v>343.9119462498504</v>
+        <v>341.8785671479067</v>
       </c>
       <c r="P25" t="n">
-        <v>365.282050632918</v>
+        <v>363.2024848338872</v>
       </c>
       <c r="Q25" t="n">
-        <v>362.6084082352801</v>
+        <v>360.4923677654069</v>
       </c>
       <c r="R25" t="n">
-        <v>384.357135478667</v>
+        <v>381.9751425278613</v>
       </c>
       <c r="S25" t="n">
-        <v>365.7468685847558</v>
+        <v>363.5542873837818</v>
       </c>
       <c r="T25" t="n">
-        <v>347.1751752493446</v>
+        <v>345.554164847468</v>
       </c>
       <c r="U25" t="n">
-        <v>349.9464062540981</v>
+        <v>347.567981030466</v>
       </c>
       <c r="V25" t="n">
-        <v>348.616590047792</v>
+        <v>346.6536563878711</v>
       </c>
       <c r="W25" t="n">
-        <v>362.5803566316529</v>
+        <v>359.987430286322</v>
       </c>
       <c r="X25" t="n">
-        <v>344.004370923516</v>
+        <v>341.5381528777924</v>
       </c>
       <c r="Y25" t="n">
-        <v>346.4332420084026</v>
+        <v>343.5390117169157</v>
       </c>
       <c r="Z25" t="n">
-        <v>336.3184647672146</v>
+        <v>333.4483872263266</v>
       </c>
       <c r="AA25" t="n">
-        <v>328.1699244217858</v>
+        <v>325.2485687781341</v>
       </c>
       <c r="AB25" t="n">
-        <v>320.434609982553</v>
+        <v>317.6849503464584</v>
       </c>
       <c r="AC25" t="n">
-        <v>320.2988556552002</v>
+        <v>317.6266650719926</v>
       </c>
       <c r="AD25" t="n">
-        <v>326.2382106349965</v>
+        <v>323.1671870877916</v>
       </c>
       <c r="AE25" t="n">
-        <v>337.749636413801</v>
+        <v>334.4469081088316</v>
       </c>
       <c r="AF25" t="n">
-        <v>344.7470391525566</v>
+        <v>341.5652942913345</v>
       </c>
       <c r="AG25" t="n">
-        <v>341.6291617751972</v>
+        <v>338.3828943419072</v>
       </c>
       <c r="AH25" t="n">
-        <v>340.534269993806</v>
+        <v>337.7063064201145</v>
       </c>
       <c r="AI25" t="n">
-        <v>341.0970905186425</v>
+        <v>338.3677240751286</v>
       </c>
       <c r="AJ25" t="n">
-        <v>338.27551264024</v>
+        <v>335.8545227249512</v>
       </c>
       <c r="AK25" t="n">
-        <v>338.1979371197063</v>
+        <v>335.8166810137178</v>
+      </c>
+      <c r="AL25" t="n">
+        <v>319.7200585341434</v>
       </c>
     </row>
     <row r="26">
@@ -3135,112 +3198,115 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>424.2721577334618</v>
+        <v>418.2143832520235</v>
       </c>
       <c r="C27" t="n">
-        <v>445.3615354323274</v>
+        <v>439.5561309424326</v>
       </c>
       <c r="D27" t="n">
-        <v>425.083987063247</v>
+        <v>419.3012591420261</v>
       </c>
       <c r="E27" t="n">
-        <v>402.4202347178407</v>
+        <v>396.684087895523</v>
       </c>
       <c r="F27" t="n">
-        <v>402.7550224678593</v>
+        <v>397.0880539267612</v>
       </c>
       <c r="G27" t="n">
-        <v>369.2561942933073</v>
+        <v>363.2085294306941</v>
       </c>
       <c r="H27" t="n">
-        <v>444.5707802377208</v>
+        <v>439.0594249847957</v>
       </c>
       <c r="I27" t="n">
-        <v>405.7001452331904</v>
+        <v>400.471009598383</v>
       </c>
       <c r="J27" t="n">
-        <v>414.5105433961123</v>
+        <v>409.0485374648179</v>
       </c>
       <c r="K27" t="n">
-        <v>413.1556468911123</v>
+        <v>407.4078080851813</v>
       </c>
       <c r="L27" t="n">
-        <v>399.2119197814841</v>
+        <v>393.7718922779271</v>
       </c>
       <c r="M27" t="n">
-        <v>410.1791812378492</v>
+        <v>404.7800368909316</v>
       </c>
       <c r="N27" t="n">
-        <v>419.81829548312</v>
+        <v>414.2874022510867</v>
       </c>
       <c r="O27" t="n">
-        <v>421.6550412329674</v>
+        <v>415.7908987522439</v>
       </c>
       <c r="P27" t="n">
-        <v>430.6999991822115</v>
+        <v>424.68935142997</v>
       </c>
       <c r="Q27" t="n">
-        <v>428.6488764710198</v>
+        <v>422.6073798620862</v>
       </c>
       <c r="R27" t="n">
-        <v>436.4354731278341</v>
+        <v>429.7154420072696</v>
       </c>
       <c r="S27" t="n">
-        <v>417.9960167978875</v>
+        <v>411.886872863352</v>
       </c>
       <c r="T27" t="n">
-        <v>398.0460342766607</v>
+        <v>393.5394985165453</v>
       </c>
       <c r="U27" t="n">
-        <v>394.2768217007849</v>
+        <v>387.6785705912972</v>
       </c>
       <c r="V27" t="n">
-        <v>398.5517187362677</v>
+        <v>393.16917438654</v>
       </c>
       <c r="W27" t="n">
-        <v>402.8746157154163</v>
+        <v>395.8464619347612</v>
       </c>
       <c r="X27" t="n">
-        <v>373.0411718179486</v>
+        <v>366.4200099336428</v>
       </c>
       <c r="Y27" t="n">
-        <v>388.8228286287175</v>
+        <v>381.1246940860984</v>
       </c>
       <c r="Z27" t="n">
-        <v>383.2750054357036</v>
+        <v>375.7081750383488</v>
       </c>
       <c r="AA27" t="n">
-        <v>376.529890631778</v>
+        <v>368.8326550550825</v>
       </c>
       <c r="AB27" t="n">
-        <v>370.2646331256685</v>
+        <v>363.0226648385928</v>
       </c>
       <c r="AC27" t="n">
-        <v>367.0689982973382</v>
+        <v>360.0510617258658</v>
       </c>
       <c r="AD27" t="n">
-        <v>387.5078133821899</v>
+        <v>379.4992426126549</v>
       </c>
       <c r="AE27" t="n">
-        <v>389.6506227053274</v>
+        <v>380.286455100577</v>
       </c>
       <c r="AF27" t="n">
-        <v>387.7036023998403</v>
+        <v>378.5456258526684</v>
       </c>
       <c r="AG27" t="n">
-        <v>379.6075202993918</v>
+        <v>370.2852108763913</v>
       </c>
       <c r="AH27" t="n">
-        <v>382.2558420079399</v>
+        <v>373.9876401170486</v>
       </c>
       <c r="AI27" t="n">
-        <v>386.6055973278106</v>
+        <v>378.5922765127253</v>
       </c>
       <c r="AJ27" t="n">
-        <v>389.4553129997065</v>
+        <v>382.2203322824454</v>
       </c>
       <c r="AK27" t="n">
-        <v>394.4301507240202</v>
+        <v>387.2692746475824</v>
+      </c>
+      <c r="AL27" t="n">
+        <v>369.0703826157091</v>
       </c>
     </row>
     <row r="28">
@@ -3369,7 +3435,10 @@
         <v>14.4738</v>
       </c>
       <c r="AK30" t="n">
-        <v>15.69927432113609</v>
+        <v>15.21916</v>
+      </c>
+      <c r="AL30" t="n">
+        <v>21.04696</v>
       </c>
     </row>
     <row r="31">
@@ -3486,6 +3555,9 @@
       <c r="AK31" t="n">
         <v>9.438733333333341</v>
       </c>
+      <c r="AL31" t="n">
+        <v>8.387866666666669</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="3" t="inlineStr">
@@ -3601,6 +3673,9 @@
       <c r="AK32" t="n">
         <v>4.23201141</v>
       </c>
+      <c r="AL32" t="n">
+        <v>3.2045607</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="3" t="inlineStr">
@@ -3616,112 +3691,115 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>-4790.406105690787</v>
+        <v>-4775.24461023306</v>
       </c>
       <c r="C34" t="n">
-        <v>-4804.027915429368</v>
+        <v>-4788.873211902914</v>
       </c>
       <c r="D34" t="n">
-        <v>-4750.136817509486</v>
+        <v>-4734.988905914305</v>
       </c>
       <c r="E34" t="n">
-        <v>-4673.425569101333</v>
+        <v>-4658.284449437425</v>
       </c>
       <c r="F34" t="n">
-        <v>-4394.558123200743</v>
+        <v>-4379.423795468108</v>
       </c>
       <c r="G34" t="n">
-        <v>-4747.576665493937</v>
+        <v>-4732.202478598209</v>
       </c>
       <c r="H34" t="n">
-        <v>-4863.685674109869</v>
+        <v>-4848.175615385426</v>
       </c>
       <c r="I34" t="n">
-        <v>-4863.807699041118</v>
+        <v>-4848.161768487961</v>
       </c>
       <c r="J34" t="n">
-        <v>-5050.254886022497</v>
+        <v>-5034.436416973947</v>
       </c>
       <c r="K34" t="n">
-        <v>-5135.995987095048</v>
+        <v>-5119.542443902237</v>
       </c>
       <c r="L34" t="n">
-        <v>-5709.28029293495</v>
+        <v>-5695.484790625811</v>
       </c>
       <c r="M34" t="n">
-        <v>-5920.839191961735</v>
+        <v>-5909.383817196399</v>
       </c>
       <c r="N34" t="n">
-        <v>-6064.379031655266</v>
+        <v>-6055.523369552434</v>
       </c>
       <c r="O34" t="n">
-        <v>-6101.297141501226</v>
+        <v>-6095.772130573293</v>
       </c>
       <c r="P34" t="n">
-        <v>-6200.753655079688</v>
+        <v>-6197.520580334917</v>
       </c>
       <c r="Q34" t="n">
-        <v>-6249.074085856345</v>
+        <v>-6248.212553560292</v>
       </c>
       <c r="R34" t="n">
-        <v>-7365.650323125661</v>
+        <v>-7367.217993074201</v>
       </c>
       <c r="S34" t="n">
-        <v>-7059.534057550612</v>
+        <v>-7045.129179126481</v>
       </c>
       <c r="T34" t="n">
-        <v>-7185.234407341679</v>
+        <v>-7190.339534461687</v>
       </c>
       <c r="U34" t="n">
-        <v>-7224.486918318968</v>
+        <v>-7230.165425851985</v>
       </c>
       <c r="V34" t="n">
-        <v>-7241.734391710678</v>
+        <v>-7214.36498376363</v>
       </c>
       <c r="W34" t="n">
-        <v>-7555.892151281372</v>
+        <v>-7560.600493669164</v>
       </c>
       <c r="X34" t="n">
-        <v>-7304.72041933706</v>
+        <v>-7308.023730639458</v>
       </c>
       <c r="Y34" t="n">
-        <v>-7239.121205979213</v>
+        <v>-7241.105111239518</v>
       </c>
       <c r="Z34" t="n">
-        <v>-7166.774106035389</v>
+        <v>-7167.58734759216</v>
       </c>
       <c r="AA34" t="n">
-        <v>-7067.696411057544</v>
+        <v>-7066.763101845038</v>
       </c>
       <c r="AB34" t="n">
-        <v>-7006.86537319538</v>
+        <v>-6991.620554894595</v>
       </c>
       <c r="AC34" t="n">
-        <v>-5307.3284190619</v>
+        <v>-5304.586333857736</v>
       </c>
       <c r="AD34" t="n">
-        <v>709.0255791390251</v>
+        <v>468.0688443435116</v>
       </c>
       <c r="AE34" t="n">
-        <v>808.4408849613832</v>
+        <v>563.3987964669641</v>
       </c>
       <c r="AF34" t="n">
-        <v>956.7345777468385</v>
+        <v>710.9011422385535</v>
       </c>
       <c r="AG34" t="n">
-        <v>949.4700362535767</v>
+        <v>706.631535760773</v>
       </c>
       <c r="AH34" t="n">
-        <v>1046.228590547508</v>
+        <v>804.429008293737</v>
       </c>
       <c r="AI34" t="n">
-        <v>-3344.820472559663</v>
+        <v>-640.744187922047</v>
       </c>
       <c r="AJ34" t="n">
-        <v>-3142.730040502018</v>
+        <v>-396.9243260138347</v>
       </c>
       <c r="AK34" t="n">
-        <v>-3105.759236315751</v>
+        <v>-320.9105003259546</v>
+      </c>
+      <c r="AL34" t="n">
+        <v>-169.3470295498522</v>
       </c>
     </row>
     <row r="35">
@@ -3758,85 +3836,88 @@
         <v>-5293.279914478772</v>
       </c>
       <c r="K35" t="n">
-        <v>-5403.548675328457</v>
+        <v>-5403.049473012907</v>
       </c>
       <c r="L35" t="n">
-        <v>-5492.217643695883</v>
+        <v>-5491.315255496833</v>
       </c>
       <c r="M35" t="n">
-        <v>-5783.319310503291</v>
+        <v>-5782.199118796041</v>
       </c>
       <c r="N35" t="n">
-        <v>-5856.98447036754</v>
+        <v>-5855.90542855974</v>
       </c>
       <c r="O35" t="n">
-        <v>-5952.839738952912</v>
+        <v>-5952.532153845912</v>
       </c>
       <c r="P35" t="n">
-        <v>-6043.251655553529</v>
+        <v>-6042.676180444554</v>
       </c>
       <c r="Q35" t="n">
-        <v>-6124.973503677925</v>
+        <v>-6124.209113121475</v>
       </c>
       <c r="R35" t="n">
-        <v>-7229.893470109035</v>
+        <v>-7228.996485432134</v>
       </c>
       <c r="S35" t="n">
-        <v>-7197.287571123356</v>
+        <v>-7178.826383662659</v>
       </c>
       <c r="T35" t="n">
-        <v>-7255.701912083929</v>
+        <v>-7255.644967273579</v>
       </c>
       <c r="U35" t="n">
-        <v>-7266.735138418357</v>
+        <v>-7266.183563503506</v>
       </c>
       <c r="V35" t="n">
-        <v>-7252.890910775855</v>
+        <v>-7218.187828906355</v>
       </c>
       <c r="W35" t="n">
-        <v>-7299.531221046072</v>
+        <v>-7299.233196016721</v>
       </c>
       <c r="X35" t="n">
-        <v>-7146.27581475381</v>
+        <v>-7145.96781399126</v>
       </c>
       <c r="Y35" t="n">
-        <v>-7143.867932267114</v>
+        <v>-7143.635580814665</v>
       </c>
       <c r="Z35" t="n">
-        <v>-7145.462245679893</v>
+        <v>-7145.454285876111</v>
       </c>
       <c r="AA35" t="n">
-        <v>-7139.937050598445</v>
+        <v>-7139.429888479113</v>
       </c>
       <c r="AB35" t="n">
-        <v>-7123.993484042517</v>
+        <v>-7117.181305233566</v>
       </c>
       <c r="AC35" t="n">
-        <v>-5359.727795796634</v>
+        <v>-5358.4484578924</v>
       </c>
       <c r="AD35" t="n">
-        <v>753.7404985803485</v>
+        <v>512.118009119934</v>
       </c>
       <c r="AE35" t="n">
-        <v>869.3221512152887</v>
+        <v>624.3746340243308</v>
       </c>
       <c r="AF35" t="n">
-        <v>989.8687361454221</v>
+        <v>742.2197539481198</v>
       </c>
       <c r="AG35" t="n">
-        <v>1106.768650469564</v>
+        <v>856.0770202589639</v>
       </c>
       <c r="AH35" t="n">
-        <v>1221.458508265157</v>
+        <v>967.5072744703369</v>
       </c>
       <c r="AI35" t="n">
-        <v>-3067.098326353372</v>
+        <v>-378.6507268435385</v>
       </c>
       <c r="AJ35" t="n">
-        <v>-3003.886303923851</v>
+        <v>-277.2229748168442</v>
       </c>
       <c r="AK35" t="n">
-        <v>-2942.223659729451</v>
+        <v>-179.9943427075618</v>
+      </c>
+      <c r="AL35" t="n">
+        <v>42.19931403756048</v>
       </c>
     </row>
     <row r="36">
@@ -3846,112 +3927,115 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>269.0608883637893</v>
+        <v>266.8620900623371</v>
       </c>
       <c r="C36" t="n">
-        <v>270.4971593257005</v>
+        <v>268.2915690929756</v>
       </c>
       <c r="D36" t="n">
-        <v>271.8207530035872</v>
+        <v>269.6083708395897</v>
       </c>
       <c r="E36" t="n">
-        <v>272.6826684867215</v>
+        <v>270.4634943914513</v>
       </c>
       <c r="F36" t="n">
-        <v>271.9444916492846</v>
+        <v>269.7185256227418</v>
       </c>
       <c r="G36" t="n">
-        <v>136.6208786517485</v>
+        <v>134.3342582086075</v>
       </c>
       <c r="H36" t="n">
-        <v>135.2629756523731</v>
+        <v>132.9978707044874</v>
       </c>
       <c r="I36" t="n">
-        <v>136.0023986985179</v>
+        <v>133.7588092458876</v>
       </c>
       <c r="J36" t="n">
-        <v>137.2048404157662</v>
+        <v>135.0194331250579</v>
       </c>
       <c r="K36" t="n">
-        <v>139.6897185296878</v>
+        <v>137.5258267342349</v>
       </c>
       <c r="L36" t="n">
-        <v>134.3601437987943</v>
+        <v>132.4917877096369</v>
       </c>
       <c r="M36" t="n">
-        <v>135.0343074960607</v>
+        <v>133.2448450384223</v>
       </c>
       <c r="N36" t="n">
-        <v>136.9342118230342</v>
+        <v>135.2230112858693</v>
       </c>
       <c r="O36" t="n">
-        <v>137.5439353458238</v>
+        <v>135.9103650180868</v>
       </c>
       <c r="P36" t="n">
-        <v>137.6255213729523</v>
+        <v>136.0689495435979</v>
       </c>
       <c r="Q36" t="n">
-        <v>140.6196092729552</v>
+        <v>139.1394042309379</v>
       </c>
       <c r="R36" t="n">
-        <v>139.5158180310747</v>
+        <v>138.1106413075373</v>
       </c>
       <c r="S36" t="n">
-        <v>155.5789096708322</v>
+        <v>154.1697032692376</v>
       </c>
       <c r="T36" t="n">
-        <v>158.55435658959</v>
+        <v>157.2012637003507</v>
       </c>
       <c r="U36" t="n">
-        <v>161.8617923980004</v>
+        <v>160.6025653973853</v>
       </c>
       <c r="V36" t="n">
-        <v>164.8369943189608</v>
+        <v>163.6360522499055</v>
       </c>
       <c r="W36" t="n">
-        <v>148.2204829986039</v>
+        <v>147.2800191206197</v>
       </c>
       <c r="X36" t="n">
-        <v>149.7372061789579</v>
+        <v>148.8749947573852</v>
       </c>
       <c r="Y36" t="n">
-        <v>151.7365404269264</v>
+        <v>150.9525814617651</v>
       </c>
       <c r="Z36" t="n">
-        <v>153.8894433530661</v>
+        <v>153.1837368443162</v>
       </c>
       <c r="AA36" t="n">
-        <v>159.1115871007043</v>
+        <v>158.4507824833525</v>
       </c>
       <c r="AB36" t="n">
-        <v>155.4020034106279</v>
+        <v>161.5452446296157</v>
       </c>
       <c r="AC36" t="n">
-        <v>172.4323201542752</v>
+        <v>171.7928065705078</v>
       </c>
       <c r="AD36" t="n">
-        <v>183.2133679724699</v>
+        <v>182.6241068012333</v>
       </c>
       <c r="AE36" t="n">
-        <v>189.1984836806975</v>
+        <v>188.6961415886583</v>
       </c>
       <c r="AF36" t="n">
-        <v>192.4189168902747</v>
+        <v>191.9227568212844</v>
       </c>
       <c r="AG36" t="n">
-        <v>150.2106900568412</v>
+        <v>149.9782868979356</v>
       </c>
       <c r="AH36" t="n">
-        <v>151.6462945138445</v>
+        <v>151.433944727525</v>
       </c>
       <c r="AI36" t="n">
-        <v>148.6890646622041</v>
+        <v>148.3980989066704</v>
       </c>
       <c r="AJ36" t="n">
-        <v>150.7375153840356</v>
+        <v>150.4046003259541</v>
       </c>
       <c r="AK36" t="n">
-        <v>149.5913779292522</v>
+        <v>149.1798469019564</v>
+      </c>
+      <c r="AL36" t="n">
+        <v>149.5361738638211</v>
       </c>
     </row>
     <row r="37">
@@ -3961,112 +4045,115 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>-302.1340910412271</v>
+        <v>-320.9228342672417</v>
       </c>
       <c r="C37" t="n">
-        <v>-304.8411901347915</v>
+        <v>-323.6299333608061</v>
       </c>
       <c r="D37" t="n">
-        <v>-283.949824228356</v>
+        <v>-302.7385674543707</v>
       </c>
       <c r="E37" t="n">
-        <v>-286.6569233219207</v>
+        <v>-305.4456665479353</v>
       </c>
       <c r="F37" t="n">
-        <v>-276.2537640821519</v>
+        <v>-295.0425073081665</v>
       </c>
       <c r="G37" t="n">
-        <v>-524.9058210354781</v>
+        <v>-543.082730884904</v>
       </c>
       <c r="H37" t="n">
-        <v>-460.4048025503482</v>
+        <v>-478.3714642966959</v>
       </c>
       <c r="I37" t="n">
-        <v>-427.2922327318823</v>
+        <v>-445.0486463751517</v>
       </c>
       <c r="J37" t="n">
-        <v>-456.5932815800828</v>
+        <v>-474.1394471202768</v>
       </c>
       <c r="K37" t="n">
-        <v>-420.1467510949503</v>
+        <v>-437.4826685320661</v>
       </c>
       <c r="L37" t="n">
-        <v>-852.3451916243415</v>
+        <v>-869.9175462584801</v>
       </c>
       <c r="M37" t="n">
-        <v>-837.5739044228316</v>
+        <v>-854.9859005049799</v>
       </c>
       <c r="N37" t="n">
-        <v>-811.164288588063</v>
+        <v>-828.415926118221</v>
       </c>
       <c r="O37" t="n">
-        <v>-781.8296959414641</v>
+        <v>-798.9209749196293</v>
       </c>
       <c r="P37" t="n">
-        <v>-742.9795274235061</v>
+        <v>-759.910447849681</v>
       </c>
       <c r="Q37" t="n">
-        <v>-717.3090318008553</v>
+        <v>-734.07959367504</v>
       </c>
       <c r="R37" t="n">
-        <v>-705.189739112149</v>
+        <v>-721.7999424343434</v>
       </c>
       <c r="S37" t="n">
-        <v>-519.8990824297671</v>
+        <v>-534.9745520192523</v>
       </c>
       <c r="T37" t="n">
-        <v>-554.1243362876928</v>
+        <v>-568.7203915051115</v>
       </c>
       <c r="U37" t="n">
-        <v>-564.3173014271716</v>
+        <v>-578.4339422725236</v>
       </c>
       <c r="V37" t="n">
-        <v>-563.4593308482038</v>
+        <v>-577.0965573214891</v>
       </c>
       <c r="W37" t="n">
-        <v>-599.3235412005865</v>
+        <v>-612.7928634150526</v>
       </c>
       <c r="X37" t="n">
-        <v>-575.0233296958731</v>
+        <v>-587.5039437043536</v>
       </c>
       <c r="Y37" t="n">
-        <v>-549.4758717671984</v>
+        <v>-560.9677775696932</v>
       </c>
       <c r="Z37" t="n">
-        <v>-520.9701035213365</v>
+        <v>-531.4733011178455</v>
       </c>
       <c r="AA37" t="n">
-        <v>-474.3532301873946</v>
+        <v>-484.0779676809963</v>
       </c>
       <c r="AB37" t="n">
-        <v>-423.5824486586609</v>
+        <v>-432.5287260493552</v>
       </c>
       <c r="AC37" t="n">
-        <v>-458.5607058130645</v>
+        <v>-466.6343464216444</v>
       </c>
       <c r="AD37" t="n">
-        <v>-458.7288586058205</v>
+        <v>-466.1864679137748</v>
       </c>
       <c r="AE37" t="n">
-        <v>-444.3932347095725</v>
+        <v>-451.2348127169013</v>
       </c>
       <c r="AF37" t="n">
-        <v>-431.8689033084047</v>
+        <v>-438.0445604640202</v>
       </c>
       <c r="AG37" t="n">
-        <v>-503.1786824057232</v>
+        <v>-508.2352702753834</v>
       </c>
       <c r="AH37" t="n">
-        <v>-471.2781868358965</v>
+        <v>-475.7338991794614</v>
       </c>
       <c r="AI37" t="n">
-        <v>-433.1627037815478</v>
+        <v>-437.4828593993017</v>
       </c>
       <c r="AJ37" t="n">
-        <v>-396.3142372838493</v>
+        <v>-400.4988361757949</v>
       </c>
       <c r="AK37" t="n">
-        <v>-356.2048934423757</v>
+        <v>-360.2539356085103</v>
+      </c>
+      <c r="AL37" t="n">
+        <v>-314.2135440612817</v>
       </c>
     </row>
     <row r="38">
@@ -4076,112 +4163,115 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>1.80610854125097</v>
+        <v>41.80106111220398</v>
       </c>
       <c r="C38" t="n">
-        <v>1.92306205736</v>
+        <v>41.91801462831304</v>
       </c>
       <c r="D38" t="n">
-        <v>2.04001557346906</v>
+        <v>42.03496814442207</v>
       </c>
       <c r="E38" t="n">
-        <v>2.15696908957809</v>
+        <v>42.15192166053113</v>
       </c>
       <c r="F38" t="n">
-        <v>2.27392260568715</v>
+        <v>42.26887517664016</v>
       </c>
       <c r="G38" t="n">
-        <v>0.81833839743696</v>
+        <v>40.83963300155917</v>
       </c>
       <c r="H38" t="n">
-        <v>0.9066744578907801</v>
+        <v>40.92738259177704</v>
       </c>
       <c r="I38" t="n">
-        <v>0.99501051834455</v>
+        <v>41.01513218199221</v>
       </c>
       <c r="J38" t="n">
-        <v>1.08334657879833</v>
+        <v>41.10288177221004</v>
       </c>
       <c r="K38" t="n">
-        <v>1.17168263925214</v>
+        <v>41.1906313624226</v>
       </c>
       <c r="L38" t="n">
-        <v>-0.9726842621148</v>
+        <v>37.35845682597838</v>
       </c>
       <c r="M38" t="n">
-        <v>-0.62197794488159</v>
+        <v>35.99058007566537</v>
       </c>
       <c r="N38" t="n">
-        <v>-0.27139796985737</v>
+        <v>34.6225769831406</v>
       </c>
       <c r="O38" t="n">
-        <v>0.07905566295774</v>
+        <v>33.25444754840938</v>
       </c>
       <c r="P38" t="n">
-        <v>0.4293829535637</v>
+        <v>31.88619177146905</v>
       </c>
       <c r="Q38" t="n">
-        <v>0.7795839019606</v>
+        <v>30.51780965231703</v>
       </c>
       <c r="R38" t="n">
-        <v>1.14418382325276</v>
+        <v>29.16382650606282</v>
       </c>
       <c r="S38" t="n">
-        <v>5.56910533115435</v>
+        <v>32.02838352567759</v>
       </c>
       <c r="T38" t="n">
-        <v>5.97815087481715</v>
+        <v>30.93476851693309</v>
       </c>
       <c r="U38" t="n">
-        <v>6.3875583216807</v>
+        <v>29.84151541138937</v>
       </c>
       <c r="V38" t="n">
-        <v>6.79732767174506</v>
+        <v>28.74862420904643</v>
       </c>
       <c r="W38" t="n">
-        <v>24.06021130002705</v>
+        <v>45.45806632702514</v>
       </c>
       <c r="X38" t="n">
-        <v>24.5755938918708</v>
+        <v>45.64441160365266</v>
       </c>
       <c r="Y38" t="n">
-        <v>25.09097648371452</v>
+        <v>45.83075688027749</v>
       </c>
       <c r="Z38" t="n">
-        <v>25.60635907555824</v>
+        <v>46.01710215690233</v>
       </c>
       <c r="AA38" t="n">
-        <v>26.12948750073529</v>
+        <v>46.21177973710174</v>
       </c>
       <c r="AB38" t="n">
-        <v>26.65261592591237</v>
+        <v>46.40645731729851</v>
       </c>
       <c r="AC38" t="n">
-        <v>-2.11383333333334</v>
+        <v>15.99316148602883</v>
       </c>
       <c r="AD38" t="n">
-        <v>-1.79978333333333</v>
+        <v>14.30131820186823</v>
       </c>
       <c r="AE38" t="n">
-        <v>-1.48573333333333</v>
+        <v>12.60947491770498</v>
       </c>
       <c r="AF38" t="n">
-        <v>-1.45857380952382</v>
+        <v>12.34873775466162</v>
       </c>
       <c r="AG38" t="n">
-        <v>20.19356949271081</v>
+        <v>36.24597507018409</v>
       </c>
       <c r="AH38" t="n">
-        <v>19.96422162772545</v>
+        <v>37.99047343281065</v>
       </c>
       <c r="AI38" t="n">
-        <v>19.92763980812449</v>
+        <v>39.79898779360702</v>
       </c>
       <c r="AJ38" t="n">
-        <v>19.8910579885235</v>
+        <v>41.60750215440342</v>
       </c>
       <c r="AK38" t="n">
-        <v>19.8544761689225</v>
+        <v>43.41601651519717</v>
+      </c>
+      <c r="AL38" t="n">
+        <v>45.22453087598827</v>
       </c>
     </row>
     <row r="39">
@@ -4191,112 +4281,115 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>463.9680256322891</v>
+        <v>459.8524592137296</v>
       </c>
       <c r="C39" t="n">
-        <v>464.2837200622766</v>
+        <v>460.1681536437171</v>
       </c>
       <c r="D39" t="n">
-        <v>464.5994144922643</v>
+        <v>460.4838480737047</v>
       </c>
       <c r="E39" t="n">
-        <v>464.9151089222519</v>
+        <v>460.7995425036924</v>
       </c>
       <c r="F39" t="n">
-        <v>465.2308033522395</v>
+        <v>461.11523693368</v>
       </c>
       <c r="G39" t="n">
-        <v>475.9054834994264</v>
+        <v>471.5367863493113</v>
       </c>
       <c r="H39" t="n">
-        <v>478.0336895602182</v>
+        <v>473.5734326990023</v>
       </c>
       <c r="I39" t="n">
-        <v>480.1618956210074</v>
+        <v>475.6100790486933</v>
       </c>
       <c r="J39" t="n">
-        <v>482.2901016817939</v>
+        <v>477.6467253983896</v>
       </c>
       <c r="K39" t="n">
-        <v>484.4183077425831</v>
+        <v>479.6833717480807</v>
       </c>
       <c r="L39" t="n">
-        <v>522.3307634533861</v>
+        <v>516.0251993012354</v>
       </c>
       <c r="M39" t="n">
-        <v>519.7713253787471</v>
+        <v>512.4644785696312</v>
       </c>
       <c r="N39" t="n">
-        <v>517.2093604599286</v>
+        <v>508.9012309938449</v>
       </c>
       <c r="O39" t="n">
-        <v>514.6448686969281</v>
+        <v>505.3354565738741</v>
       </c>
       <c r="P39" t="n">
-        <v>512.0778500897461</v>
+        <v>501.7671553097268</v>
       </c>
       <c r="Q39" t="n">
-        <v>509.5083046383791</v>
+        <v>498.1963272013921</v>
       </c>
       <c r="R39" t="n">
-        <v>507.22673864492</v>
+        <v>494.9134785509654</v>
       </c>
       <c r="S39" t="n">
-        <v>598.0549416457333</v>
+        <v>584.3490673516656</v>
       </c>
       <c r="T39" t="n">
-        <v>596.7458361458521</v>
+        <v>582.936068886303</v>
       </c>
       <c r="U39" t="n">
-        <v>595.444330613179</v>
+        <v>581.5306703881594</v>
       </c>
       <c r="V39" t="n">
-        <v>594.1504250477273</v>
+        <v>580.1328718572291</v>
       </c>
       <c r="W39" t="n">
-        <v>451.5927447801395</v>
+        <v>440.0597138595864</v>
       </c>
       <c r="X39" t="n">
-        <v>440.8017432113123</v>
+        <v>429.9131201609799</v>
       </c>
       <c r="Y39" t="n">
-        <v>430.0107416424879</v>
+        <v>419.7665264623762</v>
       </c>
       <c r="Z39" t="n">
-        <v>419.2197400736528</v>
+        <v>409.6199327637723</v>
       </c>
       <c r="AA39" t="n">
-        <v>406.1808099659879</v>
+        <v>397.3169702374262</v>
       </c>
       <c r="AB39" t="n">
-        <v>393.1418798583227</v>
+        <v>385.0140077110825</v>
       </c>
       <c r="AC39" t="n">
-        <v>351.8973937634727</v>
+        <v>344.1884796479915</v>
       </c>
       <c r="AD39" t="n">
-        <v>332.2403888295004</v>
+        <v>325.0855006370606</v>
       </c>
       <c r="AE39" t="n">
-        <v>312.5833838955255</v>
+        <v>305.9825216261323</v>
       </c>
       <c r="AF39" t="n">
-        <v>297.6418267505451</v>
+        <v>292.504713350068</v>
       </c>
       <c r="AG39" t="n">
-        <v>249.4465085233293</v>
+        <v>246.6199550352879</v>
       </c>
       <c r="AH39" t="n">
-        <v>238.7829671203323</v>
+        <v>237.5610574222343</v>
       </c>
       <c r="AI39" t="n">
-        <v>228.3121917627196</v>
+        <v>228.5661758073452</v>
       </c>
       <c r="AJ39" t="n">
-        <v>217.8414164051069</v>
+        <v>219.5712941924535</v>
       </c>
       <c r="AK39" t="n">
-        <v>207.3706410474942</v>
+        <v>210.5764125775644</v>
+      </c>
+      <c r="AL39" t="n">
+        <v>201.5815309626726</v>
       </c>
     </row>
     <row r="40">
@@ -4306,112 +4399,115 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>14.32768824318244</v>
+        <v>14.19304572613021</v>
       </c>
       <c r="C40" t="n">
-        <v>14.44464175929147</v>
+        <v>14.30999924223928</v>
       </c>
       <c r="D40" t="n">
-        <v>14.56159527540057</v>
+        <v>14.42695275834834</v>
       </c>
       <c r="E40" t="n">
-        <v>14.6785487915096</v>
+        <v>14.5439062744574</v>
       </c>
       <c r="F40" t="n">
-        <v>14.79550230761866</v>
+        <v>14.66085979056643</v>
       </c>
       <c r="G40" t="n">
-        <v>19.91823888786336</v>
+        <v>19.7028108605798</v>
       </c>
       <c r="H40" t="n">
-        <v>20.31786006649553</v>
+        <v>20.10243203921198</v>
       </c>
       <c r="I40" t="n">
-        <v>20.71748124512774</v>
+        <v>20.50205321784419</v>
       </c>
       <c r="J40" t="n">
-        <v>21.11710242375999</v>
+        <v>20.9016743964764</v>
       </c>
       <c r="K40" t="n">
-        <v>21.51672360239213</v>
+        <v>21.30129557510857</v>
       </c>
       <c r="L40" t="n">
-        <v>9.919751979224721</v>
+        <v>9.89128488980263</v>
       </c>
       <c r="M40" t="n">
-        <v>9.56070520049397</v>
+        <v>9.50377102164979</v>
       </c>
       <c r="N40" t="n">
-        <v>9.201658421763261</v>
+        <v>9.11625715349699</v>
       </c>
       <c r="O40" t="n">
-        <v>8.842611643032591</v>
+        <v>8.7287432853442</v>
       </c>
       <c r="P40" t="n">
-        <v>8.483564864301851</v>
+        <v>8.3412294171914</v>
       </c>
       <c r="Q40" t="n">
-        <v>8.12451808557114</v>
+        <v>7.95371554903857</v>
       </c>
       <c r="R40" t="n">
-        <v>7.76547130684044</v>
+        <v>7.56620168088577</v>
       </c>
       <c r="S40" t="n">
-        <v>15.80713886168705</v>
+        <v>15.46280466711348</v>
       </c>
       <c r="T40" t="n">
-        <v>15.95254584770834</v>
+        <v>15.59778960156811</v>
       </c>
       <c r="U40" t="n">
-        <v>16.09831473693034</v>
+        <v>15.73313643922352</v>
       </c>
       <c r="V40" t="n">
-        <v>16.24444552935319</v>
+        <v>15.86884518007967</v>
       </c>
       <c r="W40" t="n">
-        <v>19.03418431502943</v>
+        <v>18.61370312673845</v>
       </c>
       <c r="X40" t="n">
-        <v>19.34610263376304</v>
+        <v>18.92562144547207</v>
       </c>
       <c r="Y40" t="n">
-        <v>19.65802095249397</v>
+        <v>19.23753976420299</v>
       </c>
       <c r="Z40" t="n">
-        <v>19.96993927122493</v>
+        <v>19.54945808293396</v>
       </c>
       <c r="AA40" t="n">
-        <v>20.07440019890059</v>
+        <v>19.65391901060962</v>
       </c>
       <c r="AB40" t="n">
-        <v>20.17886112657356</v>
+        <v>19.75837993828259</v>
       </c>
       <c r="AC40" t="n">
-        <v>5.14314178746286</v>
+        <v>4.90218395524153</v>
       </c>
       <c r="AD40" t="n">
-        <v>4.58992207797504</v>
+        <v>4.3489642457537</v>
       </c>
       <c r="AE40" t="n">
-        <v>4.03670236848717</v>
+        <v>3.79574453626584</v>
       </c>
       <c r="AF40" t="n">
-        <v>4.04998682878801</v>
+        <v>3.83749608598876</v>
       </c>
       <c r="AG40" t="n">
-        <v>4.0632712890888</v>
+        <v>3.87924763571165</v>
       </c>
       <c r="AH40" t="n">
-        <v>4.0765557493896</v>
+        <v>3.92099918543457</v>
       </c>
       <c r="AI40" t="n">
-        <v>4.08984020969043</v>
+        <v>3.96275073515746</v>
       </c>
       <c r="AJ40" t="n">
-        <v>4.10312466999123</v>
+        <v>4.00450228488038</v>
       </c>
       <c r="AK40" t="n">
-        <v>4.11640913029203</v>
+        <v>4.04625383460327</v>
+      </c>
+      <c r="AL40" t="n">
+        <v>4.08800538432619</v>
       </c>
     </row>
     <row r="41">
@@ -4528,6 +4624,9 @@
       <c r="AK41" t="n">
         <v>-195.1259002976947</v>
       </c>
+      <c r="AL41" t="n">
+        <v>-304.8662880454915</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="3" t="inlineStr">
@@ -4543,112 +4642,115 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>700.014066801073</v>
+        <v>697.0143014805516</v>
       </c>
       <c r="C43" t="n">
-        <v>724.0903300041393</v>
+        <v>720.7217770527665</v>
       </c>
       <c r="D43" t="n">
-        <v>746.3039468418372</v>
+        <v>742.3757368213285</v>
       </c>
       <c r="E43" t="n">
-        <v>768.3079594675858</v>
+        <v>763.601452334993</v>
       </c>
       <c r="F43" t="n">
-        <v>773.3642035041428</v>
+        <v>769.2782538072505</v>
       </c>
       <c r="G43" t="n">
-        <v>766.5668043916234</v>
+        <v>763.2042067961079</v>
       </c>
       <c r="H43" t="n">
-        <v>732.7520182014915</v>
+        <v>727.783196882024</v>
       </c>
       <c r="I43" t="n">
-        <v>711.2519876313455</v>
+        <v>706.3913722293806</v>
       </c>
       <c r="J43" t="n">
-        <v>716.5673264890065</v>
+        <v>710.6134915507912</v>
       </c>
       <c r="K43" t="n">
-        <v>721.7620626397232</v>
+        <v>714.1152938454561</v>
       </c>
       <c r="L43" t="n">
-        <v>728.7300264429207</v>
+        <v>720.9808292121182</v>
       </c>
       <c r="M43" t="n">
-        <v>771.7228617999857</v>
+        <v>763.5849530728641</v>
       </c>
       <c r="N43" t="n">
-        <v>807.0994549910629</v>
+        <v>793.3401430406585</v>
       </c>
       <c r="O43" t="n">
-        <v>831.5956984438483</v>
+        <v>816.3538183175452</v>
       </c>
       <c r="P43" t="n">
-        <v>862.3917650622201</v>
+        <v>850.2182856801645</v>
       </c>
       <c r="Q43" t="n">
-        <v>878.9087708004463</v>
+        <v>865.9655255514695</v>
       </c>
       <c r="R43" t="n">
-        <v>871.8729078864892</v>
+        <v>857.7525163070407</v>
       </c>
       <c r="S43" t="n">
-        <v>887.5304994186477</v>
+        <v>871.6309642708972</v>
       </c>
       <c r="T43" t="n">
-        <v>888.3326887546312</v>
+        <v>866.2810156056713</v>
       </c>
       <c r="U43" t="n">
-        <v>849.2946287993742</v>
+        <v>827.9027641590042</v>
       </c>
       <c r="V43" t="n">
-        <v>809.6168716608553</v>
+        <v>775.6254029118553</v>
       </c>
       <c r="W43" t="n">
-        <v>749.2564080387008</v>
+        <v>716.7224079639008</v>
       </c>
       <c r="X43" t="n">
-        <v>673.0473922737598</v>
+        <v>642.0948847641656</v>
       </c>
       <c r="Y43" t="n">
-        <v>610.1864830367194</v>
+        <v>586.1952725208504</v>
       </c>
       <c r="Z43" t="n">
-        <v>599.1311697570312</v>
+        <v>574.1035812810715</v>
       </c>
       <c r="AA43" t="n">
-        <v>605.556934247039</v>
+        <v>585.7398386042307</v>
       </c>
       <c r="AB43" t="n">
-        <v>589.0203727297923</v>
+        <v>572.8365611917018</v>
       </c>
       <c r="AC43" t="n">
-        <v>566.9262626734283</v>
+        <v>551.3756821333326</v>
       </c>
       <c r="AD43" t="n">
-        <v>534.1337126776457</v>
+        <v>518.8798034899646</v>
       </c>
       <c r="AE43" t="n">
-        <v>542.4881740765247</v>
+        <v>531.7325471423781</v>
       </c>
       <c r="AF43" t="n">
-        <v>537.7579982671779</v>
+        <v>539.9148004035252</v>
       </c>
       <c r="AG43" t="n">
-        <v>524.2104338526574</v>
+        <v>521.7982415223353</v>
       </c>
       <c r="AH43" t="n">
-        <v>483.6548992068643</v>
+        <v>482.2445269656899</v>
       </c>
       <c r="AI43" t="n">
-        <v>474.0421765951755</v>
+        <v>463.2161402311273</v>
       </c>
       <c r="AJ43" t="n">
-        <v>451.1181149845062</v>
+        <v>440.1147896079996</v>
       </c>
       <c r="AK43" t="n">
-        <v>428.7704393738188</v>
+        <v>418.8451449858387</v>
+      </c>
+      <c r="AL43" t="n">
+        <v>380.2160669525842</v>
       </c>
     </row>
     <row r="44">
@@ -4754,16 +4856,19 @@
         <v>292.6048380212519</v>
       </c>
       <c r="AH44" t="n">
-        <v>262.0915021936688</v>
+        <v>262.0958643136688</v>
       </c>
       <c r="AI44" t="n">
-        <v>252.2075678546043</v>
+        <v>242.4625010546043</v>
       </c>
       <c r="AJ44" t="n">
-        <v>230.612598292265</v>
+        <v>218.762449492265</v>
       </c>
       <c r="AK44" t="n">
-        <v>206.288168876491</v>
+        <v>197.403278876491</v>
+      </c>
+      <c r="AL44" t="n">
+        <v>176.4784256639466</v>
       </c>
     </row>
     <row r="45">
@@ -4832,6 +4937,9 @@
       <c r="AK45" t="n">
         <v>23.0596364184</v>
       </c>
+      <c r="AL45" t="n">
+        <v>19.060502</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="7" t="inlineStr">
@@ -4945,7 +5053,10 @@
         <v>19.67186202669084</v>
       </c>
       <c r="AK46" t="n">
-        <v>14.34488268108593</v>
+        <v>14.013941837394</v>
+      </c>
+      <c r="AL46" t="n">
+        <v>14.038479690308</v>
       </c>
     </row>
     <row r="47">
@@ -4955,112 +5066,115 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>370.5536500823927</v>
+        <v>367.5538847618712</v>
       </c>
       <c r="C47" t="n">
-        <v>370.4041764246253</v>
+        <v>367.0356234732525</v>
       </c>
       <c r="D47" t="n">
-        <v>368.6325777559205</v>
+        <v>364.7043677354118</v>
       </c>
       <c r="E47" t="n">
-        <v>368.3805591207184</v>
+        <v>363.6740519881257</v>
       </c>
       <c r="F47" t="n">
-        <v>353.6804475727994</v>
+        <v>349.5944978759071</v>
       </c>
       <c r="G47" t="n">
-        <v>339.4855220141786</v>
+        <v>336.122924418663</v>
       </c>
       <c r="H47" t="n">
-        <v>317.2656636490746</v>
+        <v>312.296842329607</v>
       </c>
       <c r="I47" t="n">
-        <v>303.8124885626555</v>
+        <v>298.9518731606906</v>
       </c>
       <c r="J47" t="n">
-        <v>315.3707348568676</v>
+        <v>309.4168999186523</v>
       </c>
       <c r="K47" t="n">
-        <v>325.7988663695812</v>
+        <v>318.1520975753141</v>
       </c>
       <c r="L47" t="n">
-        <v>309.7998424579098</v>
+        <v>302.0506452271074</v>
       </c>
       <c r="M47" t="n">
-        <v>317.2428496401798</v>
+        <v>309.1049409130582</v>
       </c>
       <c r="N47" t="n">
-        <v>325.613648193638</v>
+        <v>311.8543362432336</v>
       </c>
       <c r="O47" t="n">
-        <v>321.6885815497017</v>
+        <v>306.4467014233986</v>
       </c>
       <c r="P47" t="n">
-        <v>327.3150480724959</v>
+        <v>315.1415686904404</v>
       </c>
       <c r="Q47" t="n">
-        <v>330.6977632255054</v>
+        <v>317.7545179765286</v>
       </c>
       <c r="R47" t="n">
-        <v>317.3587316430615</v>
+        <v>303.238340063613</v>
       </c>
       <c r="S47" t="n">
-        <v>323.03422055959</v>
+        <v>307.1346854118394</v>
       </c>
       <c r="T47" t="n">
-        <v>319.0080138122757</v>
+        <v>296.9563406633158</v>
       </c>
       <c r="U47" t="n">
-        <v>297.7445197163639</v>
+        <v>276.3526550759938</v>
       </c>
       <c r="V47" t="n">
-        <v>295.2497708555444</v>
+        <v>261.2583021065444</v>
       </c>
       <c r="W47" t="n">
-        <v>274.8094664998035</v>
+        <v>242.2754664250035</v>
       </c>
       <c r="X47" t="n">
-        <v>267.2652223309111</v>
+        <v>236.3127148213169</v>
       </c>
       <c r="Y47" t="n">
-        <v>259.0935690558211</v>
+        <v>235.1023585399521</v>
       </c>
       <c r="Z47" t="n">
-        <v>252.2546707175909</v>
+        <v>227.2270822416312</v>
       </c>
       <c r="AA47" t="n">
-        <v>242.8644170270075</v>
+        <v>223.0473213841993</v>
       </c>
       <c r="AB47" t="n">
-        <v>232.6164177140719</v>
+        <v>216.4326061759813</v>
       </c>
       <c r="AC47" t="n">
-        <v>218.8141082955798</v>
+        <v>203.2635277554841</v>
       </c>
       <c r="AD47" t="n">
-        <v>220.7096631473349</v>
+        <v>205.4557539596538</v>
       </c>
       <c r="AE47" t="n">
-        <v>216.1954140186302</v>
+        <v>205.4397870844836</v>
       </c>
       <c r="AF47" t="n">
-        <v>196.9494030975695</v>
+        <v>199.1062052339168</v>
       </c>
       <c r="AG47" t="n">
-        <v>186.8673632982023</v>
+        <v>184.4551709678803</v>
       </c>
       <c r="AH47" t="n">
-        <v>182.1358099904434</v>
+        <v>180.7210756292691</v>
       </c>
       <c r="AI47" t="n">
-        <v>182.0444113305299</v>
+        <v>180.9634417664817</v>
       </c>
       <c r="AJ47" t="n">
-        <v>180.9683778655504</v>
+        <v>181.8152012890438</v>
       </c>
       <c r="AK47" t="n">
-        <v>185.0777513978419</v>
+        <v>184.3682878535537</v>
+      </c>
+      <c r="AL47" t="n">
+        <v>170.6386595983297</v>
       </c>
     </row>
     <row r="48">
@@ -5199,7 +5313,10 @@
         <v>408.0597049132398</v>
       </c>
       <c r="AK52" t="n">
-        <v>309.6279725062759</v>
+        <v>309.7979146901654</v>
+      </c>
+      <c r="AL52" t="n">
+        <v>61.55052949268328</v>
       </c>
     </row>
     <row r="53">
@@ -5314,7 +5431,10 @@
         <v>26.15753281411984</v>
       </c>
       <c r="AK53" t="n">
-        <v>26.77814785523584</v>
+        <v>26.94809003912536</v>
+      </c>
+      <c r="AL53" t="n">
+        <v>61.55052949268328</v>
       </c>
     </row>
     <row r="54">
@@ -5456,6 +5576,9 @@
       <c r="AK55" t="n">
         <v>0.64359834364952</v>
       </c>
+      <c r="AL55" t="n">
+        <v>0.65245351808</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="6" t="inlineStr">
@@ -5482,7 +5605,7 @@
         <v>2450.195277350052</v>
       </c>
       <c r="H56" t="n">
-        <v>2494.406581187148</v>
+        <v>2494.406581187147</v>
       </c>
       <c r="I56" t="n">
         <v>2457.021603945134</v>
@@ -5503,10 +5626,10 @@
         <v>2774.776408416074</v>
       </c>
       <c r="O56" t="n">
-        <v>2525.283106484546</v>
+        <v>2525.283106484547</v>
       </c>
       <c r="P56" t="n">
-        <v>2575.590017483463</v>
+        <v>2575.590017483464</v>
       </c>
       <c r="Q56" t="n">
         <v>3193.632386139397</v>
@@ -5518,58 +5641,61 @@
         <v>2941.747116093454</v>
       </c>
       <c r="T56" t="n">
-        <v>2721.692259809265</v>
+        <v>2721.692259809264</v>
       </c>
       <c r="U56" t="n">
         <v>3314.753672204088</v>
       </c>
       <c r="V56" t="n">
-        <v>2921.129019623484</v>
+        <v>2921.129019623483</v>
       </c>
       <c r="W56" t="n">
-        <v>3228.117521983291</v>
+        <v>3228.117521972735</v>
       </c>
       <c r="X56" t="n">
-        <v>3420.92206566185</v>
+        <v>3420.922065613596</v>
       </c>
       <c r="Y56" t="n">
-        <v>3183.176196831102</v>
+        <v>3183.176196777518</v>
       </c>
       <c r="Z56" t="n">
-        <v>3308.009876160381</v>
+        <v>3308.009876082156</v>
       </c>
       <c r="AA56" t="n">
-        <v>3259.362510928594</v>
+        <v>3281.222564337939</v>
       </c>
       <c r="AB56" t="n">
-        <v>3191.752803537688</v>
+        <v>3220.917232159117</v>
       </c>
       <c r="AC56" t="n">
-        <v>3347.523753171223</v>
+        <v>3368.385708887096</v>
       </c>
       <c r="AD56" t="n">
-        <v>2938.418415822274</v>
+        <v>2952.35156216892</v>
       </c>
       <c r="AE56" t="n">
-        <v>3225.390548023006</v>
+        <v>3206.968081797643</v>
       </c>
       <c r="AF56" t="n">
-        <v>3210.383605733491</v>
+        <v>3181.373128679587</v>
       </c>
       <c r="AG56" t="n">
-        <v>3146.276518758636</v>
+        <v>3094.045856832944</v>
       </c>
       <c r="AH56" t="n">
-        <v>3025.182417063031</v>
+        <v>2955.380439082398</v>
       </c>
       <c r="AI56" t="n">
-        <v>2988.241796899712</v>
+        <v>2915.86086437064</v>
       </c>
       <c r="AJ56" t="n">
-        <v>2933.152090211246</v>
+        <v>2933.189631206103</v>
       </c>
       <c r="AK56" t="n">
-        <v>3221.574772124262</v>
+        <v>3221.509826564824</v>
+      </c>
+      <c r="AL56" t="n">
+        <v>2794.369407247855</v>
       </c>
     </row>
     <row r="57">
@@ -5693,6 +5819,9 @@
       <c r="AK58" t="n">
         <v>3248.981770644871</v>
       </c>
+      <c r="AL58" t="n">
+        <v>3248.996604979041</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="11" t="inlineStr">
@@ -5715,112 +5844,115 @@
         </is>
       </c>
       <c r="B61" t="n">
-        <v>20632.47421178</v>
+        <v>20638.49415171284</v>
       </c>
       <c r="C61" t="n">
-        <v>19888.09375335439</v>
+        <v>19893.94632979449</v>
       </c>
       <c r="D61" t="n">
-        <v>19353.46968034894</v>
+        <v>19358.5273230838</v>
       </c>
       <c r="E61" t="n">
-        <v>19128.04065596334</v>
+        <v>19131.50519677815</v>
       </c>
       <c r="F61" t="n">
-        <v>18797.64778314313</v>
+        <v>18802.39945278412</v>
       </c>
       <c r="G61" t="n">
-        <v>17447.82153924857</v>
+        <v>17446.78168487474</v>
       </c>
       <c r="H61" t="n">
-        <v>17432.25933601533</v>
+        <v>17434.77845142036</v>
       </c>
       <c r="I61" t="n">
-        <v>17667.81578216147</v>
+        <v>17675.70878521189</v>
       </c>
       <c r="J61" t="n">
-        <v>18082.34227232341</v>
+        <v>18080.75444339557</v>
       </c>
       <c r="K61" t="n">
-        <v>18863.25285750635</v>
+        <v>18857.18428912514</v>
       </c>
       <c r="L61" t="n">
-        <v>19463.61608208334</v>
+        <v>19445.62960958492</v>
       </c>
       <c r="M61" t="n">
-        <v>20003.94394588307</v>
+        <v>19986.37085935847</v>
       </c>
       <c r="N61" t="n">
-        <v>19600.9288834434</v>
+        <v>19575.04898970508</v>
       </c>
       <c r="O61" t="n">
-        <v>18985.92103761514</v>
+        <v>18956.06722144813</v>
       </c>
       <c r="P61" t="n">
-        <v>18769.38080744517</v>
+        <v>18736.44500365305</v>
       </c>
       <c r="Q61" t="n">
-        <v>20040.56949959349</v>
+        <v>20005.41318870762</v>
       </c>
       <c r="R61" t="n">
-        <v>20318.61467068902</v>
+        <v>20277.58814101258</v>
       </c>
       <c r="S61" t="n">
-        <v>19987.82770636113</v>
+        <v>19947.85322012075</v>
       </c>
       <c r="T61" t="n">
-        <v>20386.44313473833</v>
+        <v>20344.78195799128</v>
       </c>
       <c r="U61" t="n">
-        <v>20643.29160823714</v>
+        <v>20595.82365192981</v>
       </c>
       <c r="V61" t="n">
-        <v>20833.67346443917</v>
+        <v>20769.40879536121</v>
       </c>
       <c r="W61" t="n">
-        <v>21020.41027039119</v>
+        <v>20954.50861059587</v>
       </c>
       <c r="X61" t="n">
-        <v>21743.29269126389</v>
+        <v>21679.53038869076</v>
       </c>
       <c r="Y61" t="n">
-        <v>19566.59819158634</v>
+        <v>19510.65279981903</v>
       </c>
       <c r="Z61" t="n">
-        <v>19797.92741421541</v>
+        <v>19741.37622970888</v>
       </c>
       <c r="AA61" t="n">
-        <v>19716.01103075885</v>
+        <v>19667.90550923412</v>
       </c>
       <c r="AB61" t="n">
-        <v>19083.13755320007</v>
+        <v>19038.51520316368</v>
       </c>
       <c r="AC61" t="n">
-        <v>18382.00457813237</v>
+        <v>18339.14144828748</v>
       </c>
       <c r="AD61" t="n">
-        <v>16726.12333399195</v>
+        <v>16678.66984457936</v>
       </c>
       <c r="AE61" t="n">
-        <v>16912.46539968917</v>
+        <v>16866.39948027183</v>
       </c>
       <c r="AF61" t="n">
-        <v>17790.02676668252</v>
+        <v>17751.62449121275</v>
       </c>
       <c r="AG61" t="n">
-        <v>17870.42776628583</v>
+        <v>17827.77898618812</v>
       </c>
       <c r="AH61" t="n">
-        <v>17689.13065218693</v>
+        <v>17645.98388550558</v>
       </c>
       <c r="AI61" t="n">
-        <v>17204.82660180772</v>
+        <v>17151.95244209484</v>
       </c>
       <c r="AJ61" t="n">
-        <v>15974.78348838834</v>
+        <v>15929.76668733088</v>
       </c>
       <c r="AK61" t="n">
-        <v>16106.47722729196</v>
+        <v>16073.58881333814</v>
+      </c>
+      <c r="AL61" t="n">
+        <v>15615.08725425512</v>
       </c>
     </row>
     <row r="62">
@@ -5830,112 +5962,115 @@
         </is>
       </c>
       <c r="B62" t="n">
-        <v>15842.06810608921</v>
+        <v>15863.24954147978</v>
       </c>
       <c r="C62" t="n">
-        <v>15084.06583792503</v>
+        <v>15105.07311789158</v>
       </c>
       <c r="D62" t="n">
-        <v>14603.33286283946</v>
+        <v>14623.53841716949</v>
       </c>
       <c r="E62" t="n">
-        <v>14454.61508686201</v>
+        <v>14473.22074734073</v>
       </c>
       <c r="F62" t="n">
-        <v>14403.08965994239</v>
+        <v>14422.97565731601</v>
       </c>
       <c r="G62" t="n">
-        <v>12700.24487375463</v>
+        <v>12714.57920627653</v>
       </c>
       <c r="H62" t="n">
-        <v>12568.57366190546</v>
+        <v>12586.60283603493</v>
       </c>
       <c r="I62" t="n">
-        <v>12804.00808312036</v>
+        <v>12827.54701672393</v>
       </c>
       <c r="J62" t="n">
-        <v>13032.08738630091</v>
+        <v>13046.31802642162</v>
       </c>
       <c r="K62" t="n">
-        <v>13727.2568704113</v>
+        <v>13737.6418452229</v>
       </c>
       <c r="L62" t="n">
-        <v>13754.33578914839</v>
+        <v>13750.14481895911</v>
       </c>
       <c r="M62" t="n">
-        <v>14083.10475392134</v>
+        <v>14076.98704216207</v>
       </c>
       <c r="N62" t="n">
-        <v>13536.54985178814</v>
+        <v>13519.52562015265</v>
       </c>
       <c r="O62" t="n">
-        <v>12884.62389611392</v>
+        <v>12860.29509087484</v>
       </c>
       <c r="P62" t="n">
-        <v>12568.62715236548</v>
+        <v>12538.92442331814</v>
       </c>
       <c r="Q62" t="n">
-        <v>13791.49541373714</v>
+        <v>13757.20063514733</v>
       </c>
       <c r="R62" t="n">
-        <v>12952.96434756336</v>
+        <v>12910.37014793839</v>
       </c>
       <c r="S62" t="n">
-        <v>12928.29364881052</v>
+        <v>12902.72404099427</v>
       </c>
       <c r="T62" t="n">
-        <v>13201.20872739665</v>
+        <v>13154.4424235296</v>
       </c>
       <c r="U62" t="n">
-        <v>13418.80468991817</v>
+        <v>13365.65822607783</v>
       </c>
       <c r="V62" t="n">
-        <v>13591.93907272849</v>
+        <v>13555.04381159758</v>
       </c>
       <c r="W62" t="n">
-        <v>13464.51811910982</v>
+        <v>13393.90811692671</v>
       </c>
       <c r="X62" t="n">
-        <v>14438.57227192683</v>
+        <v>14371.5066580513</v>
       </c>
       <c r="Y62" t="n">
-        <v>12327.47698560713</v>
+        <v>12269.54768857951</v>
       </c>
       <c r="Z62" t="n">
-        <v>12631.15330818002</v>
+        <v>12573.78888211672</v>
       </c>
       <c r="AA62" t="n">
-        <v>12648.3146197013</v>
+        <v>12601.14240738908</v>
       </c>
       <c r="AB62" t="n">
-        <v>12076.27218000469</v>
+        <v>12046.89464826908</v>
       </c>
       <c r="AC62" t="n">
-        <v>13074.67615907047</v>
+        <v>13034.55511442974</v>
       </c>
       <c r="AD62" t="n">
-        <v>17435.14891313097</v>
+        <v>17146.73868892287</v>
       </c>
       <c r="AE62" t="n">
-        <v>17720.90628465055</v>
+        <v>17429.79827673879</v>
       </c>
       <c r="AF62" t="n">
-        <v>18746.76134442936</v>
+        <v>18462.52563345131</v>
       </c>
       <c r="AG62" t="n">
-        <v>18819.89780253941</v>
+        <v>18534.4105219489</v>
       </c>
       <c r="AH62" t="n">
-        <v>18735.35924273444</v>
+        <v>18450.41289379931</v>
       </c>
       <c r="AI62" t="n">
-        <v>13860.00612924806</v>
+        <v>16511.20825417279</v>
       </c>
       <c r="AJ62" t="n">
-        <v>12832.05344788632</v>
+        <v>15532.84236131705</v>
       </c>
       <c r="AK62" t="n">
-        <v>13000.71799097621</v>
+        <v>15752.67831301219</v>
+      </c>
+      <c r="AL62" t="n">
+        <v>15445.74022470527</v>
       </c>
     </row>
     <row r="63">

</xml_diff>